<commit_message>
updates on final problem 1 (finished first pass at it)
</commit_message>
<xml_diff>
--- a/CS-513/FinalExam/final_problem1.xlsx
+++ b/CS-513/FinalExam/final_problem1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyatthenryblair/Desktop/Projects/Stevens/CS-513/FinalExam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE797F-9330-BF4D-BDC8-77CFF132866F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4205589-2844-5B45-A4E2-760B9C98F47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{5CD4EC78-82A5-1D4F-B2C7-988FE798375A}"/>
+    <workbookView xWindow="1100" yWindow="840" windowWidth="28040" windowHeight="17420" xr2:uid="{5CD4EC78-82A5-1D4F-B2C7-988FE798375A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="62">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -86,6 +108,9 @@
     <t>PROBLEM 1)</t>
   </si>
   <si>
+    <t>Proportion</t>
+  </si>
+  <si>
     <t>Black-Old</t>
   </si>
   <si>
@@ -110,6 +135,9 @@
     <t>Gini</t>
   </si>
   <si>
+    <t>Count</t>
+  </si>
+  <si>
     <t>Class</t>
   </si>
   <si>
@@ -171,13 +199,58 @@
   </si>
   <si>
     <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Total Entropy</t>
+  </si>
+  <si>
+    <t>log2(Proportion)</t>
+  </si>
+  <si>
+    <t>Proportion-Alcohol</t>
+  </si>
+  <si>
+    <t>Proportion-Cocaine</t>
+  </si>
+  <si>
+    <t>Proportion-Heroin</t>
+  </si>
+  <si>
+    <t>log2(Proportion-Alcohol)</t>
+  </si>
+  <si>
+    <t>log2(Proportion-Cocaine)</t>
+  </si>
+  <si>
+    <t>log2(Proportion-Heroin)</t>
+  </si>
+  <si>
+    <t>Information Gain</t>
+  </si>
+  <si>
+    <t>Entropy-LEFT</t>
+  </si>
+  <si>
+    <t>Entropy-RIGHT</t>
+  </si>
+  <si>
+    <t>Split Count</t>
+  </si>
+  <si>
+    <t>&lt;-- Highest Information Gain is if we split on Age</t>
+  </si>
+  <si>
+    <t>&lt;-- Highest Information Gain is if we split on Black / not Black</t>
+  </si>
+  <si>
+    <t>--&gt; Identical to 1.a)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,6 +306,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +418,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -347,8 +440,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -409,6 +520,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -430,6 +552,19 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,14 +591,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -489,38 +699,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
@@ -528,7 +759,323 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -591,6 +1138,151 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{AA030ACC-6FD3-EE48-A815-BAE7DF96757E}" name="Table2934" displayName="Table2934" ref="A114:D117" totalsRowShown="0">
+  <autoFilter ref="A114:D117" xr:uid="{AA030ACC-6FD3-EE48-A815-BAE7DF96757E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1AF29117-07FE-BC47-8BED-471103CE1F23}" name="Class"/>
+    <tableColumn id="2" xr3:uid="{ED43A0C6-BDE5-4744-A513-775D6ECE5DDC}" name="Count">
+      <calculatedColumnFormula>C111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{5E2E1EF9-CA94-0447-A499-CEE3674B13D3}" name="Proportion">
+      <calculatedColumnFormula>Table2934[[#This Row],[Count]]/$F$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{64DCBBF0-FA2B-D540-A32F-D2E80DFBD8D6}" name="log2(Proportion)">
+      <calculatedColumnFormula>LOG(Table2934[[#This Row],[Proportion]], 2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{75BBD0AB-39EE-C441-B43B-C97FDAFA1816}" name="Table3035" displayName="Table3035" ref="A121:H124" totalsRowShown="0">
+  <autoFilter ref="A121:H124" xr:uid="{75BBD0AB-39EE-C441-B43B-C97FDAFA1816}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8D486482-DF28-5049-AA4E-AF8DBFC046DA}" name="Possible Split" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{9BAEBEB2-5B4A-B149-96EF-E5DB45F8330F}" name="Proportion-Alcohol">
+      <calculatedColumnFormula>C108/$F$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{953A956B-F1AF-3940-ABF8-6374F591F1CA}" name="Proportion-Cocaine">
+      <calculatedColumnFormula>D108/$F$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{7F2F7CCB-AC3C-6A4C-A941-812211704515}" name="Proportion-Heroin">
+      <calculatedColumnFormula>E108/$F$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{DF257C27-0C9D-D94B-9FD7-262D00C7A5B8}" name="log2(Proportion-Alcohol)">
+      <calculatedColumnFormula>LOG(Table3035[[#This Row],[Proportion-Alcohol]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C5419759-3651-5945-9CF7-4F5AB27B0358}" name="log2(Proportion-Cocaine)">
+      <calculatedColumnFormula>LOG(Table3035[[#This Row],[Proportion-Cocaine]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{8E4B4878-660E-9846-8ED2-9F7C5C358BB6}" name="log2(Proportion-Heroin)">
+      <calculatedColumnFormula>LOG(Table3035[[#This Row],[Proportion-Heroin]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{C45EEF6E-41C4-D644-BABC-646144C6E887}" name="Split Count">
+      <calculatedColumnFormula>F108</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{D5953D6F-FB9F-264F-AC79-0695F35359AD}" name="Table35" displayName="Table35" ref="A126:D129" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="A126:D129" xr:uid="{D5953D6F-FB9F-264F-AC79-0695F35359AD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8D16C576-2D75-A54C-8427-4BE82FC6F7DD}" name="Possible Split"/>
+    <tableColumn id="2" xr3:uid="{8A308947-5145-A042-96C6-12D3867C7CF6}" name="Entropy-LEFT" dataDxfId="9">
+      <calculatedColumnFormula array="1">-SUM(B122:D122*E122:G122)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{44A464E1-0A52-F149-8F96-FA1A7ECD8993}" name="Entropy-RIGHT"/>
+    <tableColumn id="4" xr3:uid="{4855F0AF-3A2B-9E45-821C-63A25EAD374F}" name="Information Gain" dataDxfId="8">
+      <calculatedColumnFormula>$B$119 - ((H122/$F$111) * B127 + (($F$111-H122)/$F$111) * C127)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{AB38797A-1D3F-4348-915B-B0889658CBD1}" name="Table293437" displayName="Table293437" ref="K114:N117" totalsRowShown="0">
+  <autoFilter ref="K114:N117" xr:uid="{AB38797A-1D3F-4348-915B-B0889658CBD1}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{64E35CA9-40A1-A048-945B-19BB579DDEE7}" name="Class"/>
+    <tableColumn id="2" xr3:uid="{545B5759-FA07-D841-A059-BCCCD4F5462E}" name="Count">
+      <calculatedColumnFormula>M111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{DBAAFA90-FAE4-FE4D-B6DD-862171A5D0E0}" name="Proportion">
+      <calculatedColumnFormula>Table293437[[#This Row],[Count]]/$P$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{20CE7502-C7D4-A941-BB54-EEE60DF16623}" name="log2(Proportion)">
+      <calculatedColumnFormula>LOG(Table293437[[#This Row],[Proportion]], 2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{AEEAF083-94C5-E040-97B5-B006E6DE8E9E}" name="Table303538" displayName="Table303538" ref="K121:R124" totalsRowShown="0">
+  <autoFilter ref="K121:R124" xr:uid="{AEEAF083-94C5-E040-97B5-B006E6DE8E9E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{76339E86-038F-1A43-A8BF-8366E8692653}" name="Possible Split" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{31587502-7DC9-7B4A-9B30-039493AE76BD}" name="Proportion-Alcohol">
+      <calculatedColumnFormula>M108/$P$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B8EF5723-76AC-2548-9E53-A3FDAFD6DEBD}" name="Proportion-Cocaine">
+      <calculatedColumnFormula>N108/$P$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E6DE2B93-39F4-1A42-8DC5-456A135D1422}" name="Proportion-Heroin">
+      <calculatedColumnFormula>O108/$P$111</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{5BD5F7E3-6519-EB44-8B7F-3EABA23EDC4E}" name="log2(Proportion-Alcohol)">
+      <calculatedColumnFormula>LOG(Table303538[[#This Row],[Proportion-Alcohol]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5CF069B4-DD25-1848-A7C8-2248DC5568EF}" name="log2(Proportion-Cocaine)">
+      <calculatedColumnFormula>LOG(Table303538[[#This Row],[Proportion-Cocaine]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{BDE45C28-B8EB-CD40-944A-F41DE00E2F53}" name="log2(Proportion-Heroin)">
+      <calculatedColumnFormula>LOG(Table303538[[#This Row],[Proportion-Heroin]], 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{23040BA9-9215-7B43-B9C8-098CF4A87409}" name="Split Count">
+      <calculatedColumnFormula>P108</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{6F100573-32FC-7E4E-BC13-4C639F7894F7}" name="Table3539" displayName="Table3539" ref="K126:N129" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="K126:N129" xr:uid="{6F100573-32FC-7E4E-BC13-4C639F7894F7}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C02457B7-66AA-EA42-8451-1EFFF213F3DB}" name="Possible Split"/>
+    <tableColumn id="2" xr3:uid="{B618B80B-0276-D249-9088-486929EA9DF1}" name="Entropy-LEFT" dataDxfId="1">
+      <calculatedColumnFormula array="1">-SUM(L122:N122*O122:Q122)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E66A36CC-201B-2247-B720-5585DDDBF2F9}" name="Entropy-RIGHT"/>
+    <tableColumn id="4" xr3:uid="{26CCF05E-437A-E545-98B2-A8CC4ECCC6A2}" name="Information Gain" dataDxfId="0">
+      <calculatedColumnFormula>$L$119 - ((R122/$P$111) * L127 + (($P$111-R122)/$P$111) * M127)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{385271F4-FBCE-B644-87ED-881EB4EEF53F}" name="Table2746" displayName="Table2746" ref="A148:B154" totalsRowShown="0">
+  <autoFilter ref="A148:B154" xr:uid="{385271F4-FBCE-B644-87ED-881EB4EEF53F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{216BE0B6-311E-BC47-92B5-C2A655A4E306}" name="Features"/>
+    <tableColumn id="2" xr3:uid="{D9A3A217-67A9-3B4A-912E-2E348883C580}" name="Prediction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1B3216BD-1045-FD42-B080-141593B8DFD2}" name="Table22" displayName="Table22" ref="A25:H30" totalsRowShown="0">
   <autoFilter ref="A25:H30" xr:uid="{1B3216BD-1045-FD42-B080-141593B8DFD2}"/>
@@ -608,7 +1300,7 @@
     <tableColumn id="7" xr3:uid="{0F3398B9-6D8B-7441-A481-451F38EB45EF}" name="P(Heroin | Split)">
       <calculatedColumnFormula>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B764E740-4892-DF48-8B12-44BC35B38363}" name="Gini" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{B764E740-4892-DF48-8B12-44BC35B38363}" name="Gini" dataDxfId="19">
       <calculatedColumnFormula>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -646,7 +1338,7 @@
     <tableColumn id="7" xr3:uid="{AC286A11-D77B-E340-BA31-B4D6E9643321}" name="P(Heroin | Split)">
       <calculatedColumnFormula>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C900C692-5705-1A40-9E9E-1F7DA2253954}" name="Gini" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{C900C692-5705-1A40-9E9E-1F7DA2253954}" name="Gini" dataDxfId="18">
       <calculatedColumnFormula>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -688,7 +1380,7 @@
     <tableColumn id="7" xr3:uid="{8CA111E9-A28F-6F4A-8FBC-E75109C64BC0}" name="P(Heroin | Split)">
       <calculatedColumnFormula>Table222527[[#This Row],[Count-Heroin]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F10DBE61-3A1C-5F45-82BE-7606E7A3A046}" name="Gini" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{F10DBE61-3A1C-5F45-82BE-7606E7A3A046}" name="Gini" dataDxfId="17">
       <calculatedColumnFormula>1 - SUMSQ(Table222527[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -702,6 +1394,49 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{686375EA-BFF0-FB4B-8961-23387DECD21C}" name="Features"/>
     <tableColumn id="2" xr3:uid="{33858CC2-51B2-D148-B483-44C4BED68B74}" name="Prediction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{3A7F5C9A-77DA-9046-B924-5B683B502114}" name="Table29" displayName="Table29" ref="A90:D93" totalsRowShown="0">
+  <autoFilter ref="A90:D93" xr:uid="{3A7F5C9A-77DA-9046-B924-5B683B502114}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1E7F6FB2-8A84-F947-8407-BD4A35C0A73F}" name="Class"/>
+    <tableColumn id="2" xr3:uid="{41FB35BC-553D-1B43-B375-05BE69BFC931}" name="Count">
+      <calculatedColumnFormula>C87</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{50F15CD9-D240-414B-A030-A24E758DE60C}" name="Proportion">
+      <calculatedColumnFormula>Table29[[#This Row],[Count]]/$F$87</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{C8765CC0-8083-4A48-8076-6B50D92FB76F}" name="log2(Proportion)">
+      <calculatedColumnFormula>LOG(Table29[[#This Row],[Proportion]], 2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{6A3A5B08-3666-D645-BC31-B575D97AC0F7}" name="Table30" displayName="Table30" ref="A97:K102" totalsRowShown="0">
+  <autoFilter ref="A97:K102" xr:uid="{6A3A5B08-3666-D645-BC31-B575D97AC0F7}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{C10FA415-890A-1148-9322-020408D738AF}" name="Possible Split" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{9EBDA401-A229-4A48-B7D7-1ED70BEC007C}" name="Proportion-Alcohol"/>
+    <tableColumn id="3" xr3:uid="{3DCDF509-2C30-1949-87A7-C73FDF0E39F1}" name="Proportion-Cocaine"/>
+    <tableColumn id="4" xr3:uid="{A974C6BF-01C6-3149-82B0-497F9FA26C8D}" name="Proportion-Heroin"/>
+    <tableColumn id="5" xr3:uid="{72BB6A70-AFD5-8B44-BB0B-6FE9915859E4}" name="log2(Proportion-Alcohol)"/>
+    <tableColumn id="6" xr3:uid="{E6348F1E-0956-DA46-8D51-4776FE215E88}" name="log2(Proportion-Cocaine)"/>
+    <tableColumn id="7" xr3:uid="{970A11B3-C931-9941-B90B-A254361ACC46}" name="log2(Proportion-Heroin)"/>
+    <tableColumn id="11" xr3:uid="{47910805-D1F0-D646-A837-08DBF1C7B570}" name="Split Count"/>
+    <tableColumn id="8" xr3:uid="{9DBB39E3-3F14-254F-B4E6-77C30BF041E1}" name="Entropy-LEFT" dataDxfId="15">
+      <calculatedColumnFormula array="1">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{FCB7C860-FD19-5F46-AC67-19B44F71F740}" name="Entropy-RIGHT" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{12925CAA-2661-964A-835C-C5D1843BD7D7}" name="Information Gain">
+      <calculatedColumnFormula>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1004,25 +1739,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E81D6DC-F462-584B-94C4-8AECFCC18FE7}">
-  <dimension ref="A1:S78"/>
+  <dimension ref="A1:S154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="44.33203125" customWidth="1"/>
-    <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="28" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" customWidth="1"/>
+    <col min="16" max="16" width="27.83203125" customWidth="1"/>
+    <col min="17" max="17" width="32.33203125" customWidth="1"/>
     <col min="18" max="18" width="16.6640625" customWidth="1"/>
     <col min="19" max="19" width="17.6640625" customWidth="1"/>
     <col min="21" max="21" width="10.83203125" customWidth="1"/>
@@ -1033,40 +1774,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="M1" s="9"/>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="A2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
       <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1258,16 +1999,16 @@
       <c r="M14" s="9"/>
     </row>
     <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -1298,74 +2039,74 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="A23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="13">
         <f>1 - (B19^2 + B20^2 + B21^2)</f>
         <v>0.65823750000000003</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="16">
         <f>C6+C7</f>
         <v>55</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="16">
         <f>D6+D7</f>
         <v>120</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="16">
         <f>E6+E7</f>
         <v>30</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="17">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.26829268292682928</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="17">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.58536585365853655</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="17">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.14634146341463414</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="18">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.56395002974419994</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -1384,19 +2125,19 @@
         <f>E8+E9</f>
         <v>24</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="15">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32608695652173914</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="15">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.15217391304347827</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="15">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="14">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.59829867674858228</v>
       </c>
@@ -1417,19 +2158,19 @@
         <f>E10+E11</f>
         <v>51</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="15">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.57718120805369133</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="15">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>8.0536912751677847E-2</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="15">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.34228187919463088</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="14">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.54321877392910223</v>
       </c>
@@ -1450,19 +2191,19 @@
         <f>E6+E8+E10</f>
         <v>39</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="15">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.521505376344086</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="15">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.26881720430107525</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="15">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.20967741935483872</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="14">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.61180483292866228</v>
       </c>
@@ -1483,54 +2224,54 @@
         <f>E7+E9+E11</f>
         <v>66</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="15">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.27570093457943923</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="15">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.41588785046728971</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="15">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.30841121495327101</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H30" s="14">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.65590881299676829</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="E31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="32"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="34"/>
     </row>
     <row r="33" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="22"/>
-      <c r="K33" s="29" t="s">
-        <v>35</v>
+      <c r="A33" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" s="23"/>
+      <c r="K33" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
@@ -1557,7 +2298,7 @@
       <c r="F34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="22"/>
+      <c r="I34" s="23"/>
       <c r="K34" s="4" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +2338,7 @@
         <f>SUM(C35:E35)</f>
         <v>95</v>
       </c>
-      <c r="I35" s="22"/>
+      <c r="I35" s="23"/>
       <c r="K35" s="4" t="s">
         <v>9</v>
       </c>
@@ -1636,7 +2377,7 @@
         <f t="shared" ref="F36" si="3">SUM(C36:E36)</f>
         <v>110</v>
       </c>
-      <c r="I36" s="22"/>
+      <c r="I36" s="23"/>
       <c r="K36" s="4"/>
       <c r="L36" s="5" t="s">
         <v>8</v>
@@ -1676,7 +2417,7 @@
         <f>SUM(C35:E36)</f>
         <v>205</v>
       </c>
-      <c r="I37" s="22"/>
+      <c r="I37" s="23"/>
       <c r="K37" s="4" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +2439,7 @@
       </c>
     </row>
     <row r="38" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="22"/>
+      <c r="I38" s="23"/>
       <c r="K38" s="4"/>
       <c r="L38" s="5" t="s">
         <v>8</v>
@@ -1718,7 +2459,7 @@
       </c>
     </row>
     <row r="39" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="22"/>
+      <c r="I39" s="23"/>
       <c r="K39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1741,21 +2482,21 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I40" s="22"/>
+      <c r="I40" s="23"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="I41" s="22"/>
+        <v>27</v>
+      </c>
+      <c r="I41" s="23"/>
       <c r="K41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L41" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -1766,7 +2507,7 @@
         <f>$C$37/$F$37</f>
         <v>0.26829268292682928</v>
       </c>
-      <c r="I42" s="22"/>
+      <c r="I42" s="23"/>
       <c r="K42" t="s">
         <v>2</v>
       </c>
@@ -1783,7 +2524,7 @@
         <f>$D$37/$F$37</f>
         <v>0.58536585365853655</v>
       </c>
-      <c r="I43" s="22"/>
+      <c r="I43" s="23"/>
       <c r="K43" t="s">
         <v>3</v>
       </c>
@@ -1800,7 +2541,7 @@
         <f>$E$37/$F$37</f>
         <v>0.14634146341463414</v>
       </c>
-      <c r="I44" s="22"/>
+      <c r="I44" s="23"/>
       <c r="K44" t="s">
         <v>4</v>
       </c>
@@ -1810,77 +2551,77 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I45" s="22"/>
+      <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="12">
+      <c r="A46" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="13">
         <f>1 - SUMSQ(Table212426[P(Class)])</f>
         <v>0.56395002974419994</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="K46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L46" s="12">
+      <c r="I46" s="23"/>
+      <c r="K46" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L46" s="13">
         <f>1 - SUMSQ(Table2124[P(Class)])</f>
         <v>0.57430637738330037</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I47" s="28"/>
+      <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="23"/>
+      <c r="K48" t="s">
         <v>28</v>
       </c>
-      <c r="D48" t="s">
+      <c r="L48" t="s">
         <v>29</v>
       </c>
-      <c r="E48" t="s">
+      <c r="M48" t="s">
         <v>30</v>
       </c>
-      <c r="F48" t="s">
+      <c r="N48" t="s">
         <v>31</v>
       </c>
-      <c r="G48" t="s">
+      <c r="O48" t="s">
         <v>32</v>
       </c>
-      <c r="H48" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="22"/>
-      <c r="K48" t="s">
-        <v>26</v>
-      </c>
-      <c r="L48" t="s">
-        <v>27</v>
-      </c>
-      <c r="M48" t="s">
-        <v>28</v>
-      </c>
-      <c r="N48" t="s">
-        <v>29</v>
-      </c>
-      <c r="O48" t="s">
-        <v>30</v>
-      </c>
       <c r="P48" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q48" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
@@ -1899,23 +2640,23 @@
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="15">
         <f>Table222527[[#This Row],[Count-Alcohol]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.31578947368421051</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="15">
         <f>Table222527[[#This Row],[Count-Cocaine]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.50526315789473686</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="15">
         <f>Table222527[[#This Row],[Count-Heroin]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.17894736842105263</v>
       </c>
-      <c r="H49" s="13">
+      <c r="H49" s="14">
         <f>1 - SUMSQ(Table222527[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.61296398891966764</v>
       </c>
-      <c r="I49" s="28"/>
+      <c r="I49" s="30"/>
       <c r="K49" t="s">
         <v>9</v>
       </c>
@@ -1931,58 +2672,58 @@
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="O49" s="14">
+      <c r="O49" s="15">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32608695652173914</v>
       </c>
-      <c r="P49" s="14">
+      <c r="P49" s="15">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.15217391304347827</v>
       </c>
-      <c r="Q49" s="14">
+      <c r="Q49" s="15">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="R49" s="13">
+      <c r="R49" s="14">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.59829867674858228</v>
       </c>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="16">
         <f>C36</f>
         <v>25</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="16">
         <f t="shared" ref="C50:D50" si="6">D36</f>
         <v>72</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="16">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E50" s="17">
         <f>Table222527[[#This Row],[Count-Alcohol]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.22727272727272727</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F50" s="17">
         <f>Table222527[[#This Row],[Count-Cocaine]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.65454545454545454</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G50" s="17">
         <f>Table222527[[#This Row],[Count-Heroin]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.11818181818181818</v>
       </c>
-      <c r="H50" s="17">
+      <c r="H50" s="18">
         <f>1 - SUMSQ(Table222527[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.50595041322314049</v>
       </c>
-      <c r="I50" s="28" t="s">
-        <v>37</v>
+      <c r="I50" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="K50" t="s">
         <v>10</v>
@@ -1999,62 +2740,62 @@
         <f t="shared" si="7"/>
         <v>51</v>
       </c>
-      <c r="O50" s="14">
+      <c r="O50" s="15">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.57718120805369133</v>
       </c>
-      <c r="P50" s="14">
+      <c r="P50" s="15">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>8.0536912751677847E-2</v>
       </c>
-      <c r="Q50" s="14">
+      <c r="Q50" s="15">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.34228187919463088</v>
       </c>
-      <c r="R50" s="13">
+      <c r="R50" s="14">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.54321877392910223</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I51" s="22"/>
-      <c r="K51" s="15" t="s">
+      <c r="I51" s="23"/>
+      <c r="K51" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L51" s="15">
+      <c r="L51" s="16">
         <f>M35+M37</f>
         <v>67</v>
       </c>
-      <c r="M51" s="15">
+      <c r="M51" s="16">
         <f t="shared" ref="M51:N51" si="8">N35+N37</f>
         <v>2</v>
       </c>
-      <c r="N51" s="15">
+      <c r="N51" s="16">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="O51" s="16">
+      <c r="O51" s="17">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.73626373626373631</v>
       </c>
-      <c r="P51" s="16">
+      <c r="P51" s="17">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>2.197802197802198E-2</v>
       </c>
-      <c r="Q51" s="16">
+      <c r="Q51" s="17">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.24175824175824176</v>
       </c>
-      <c r="R51" s="17">
+      <c r="R51" s="18">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.3989856297548604</v>
       </c>
       <c r="S51" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I52" s="22"/>
+      <c r="I52" s="23"/>
       <c r="K52" t="s">
         <v>8</v>
       </c>
@@ -2070,49 +2811,49 @@
         <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="O52" s="14">
+      <c r="O52" s="15">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32692307692307693</v>
       </c>
-      <c r="P52" s="14">
+      <c r="P52" s="15">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.16346153846153846</v>
       </c>
-      <c r="Q52" s="14">
+      <c r="Q52" s="15">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.50961538461538458</v>
       </c>
-      <c r="R52" s="13">
+      <c r="R52" s="14">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.60669378698224852</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I53" s="22"/>
+      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="31"/>
-      <c r="M54" s="31"/>
-      <c r="N54" s="31"/>
-      <c r="O54" s="31"/>
-      <c r="P54" s="32"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="34"/>
     </row>
     <row r="55" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="29" t="s">
-        <v>34</v>
+      <c r="A55" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2121,10 +2862,10 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
-      <c r="I55" s="22"/>
+      <c r="I55" s="23"/>
       <c r="J55" s="10"/>
-      <c r="K55" s="29" t="s">
-        <v>34</v>
+      <c r="K55" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
@@ -2142,7 +2883,7 @@
       <c r="C56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="27" t="s">
+      <c r="D56" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2151,14 +2892,14 @@
       <c r="F56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I56" s="22"/>
+      <c r="I56" s="23"/>
       <c r="K56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M56" s="27" t="s">
+      <c r="M56" s="29" t="s">
         <v>2</v>
       </c>
       <c r="N56" s="3" t="s">
@@ -2181,7 +2922,7 @@
       <c r="C57" s="6">
         <v>25</v>
       </c>
-      <c r="D57" s="21">
+      <c r="D57" s="22">
         <v>72</v>
       </c>
       <c r="E57" s="6">
@@ -2191,14 +2932,14 @@
         <f t="shared" ref="F57" si="10">SUM(C57:E57)</f>
         <v>110</v>
       </c>
-      <c r="I57" s="22"/>
+      <c r="I57" s="23"/>
       <c r="K57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M57" s="21">
+      <c r="M57" s="22">
         <v>7</v>
       </c>
       <c r="N57" s="6">
@@ -2221,7 +2962,7 @@
         <f>SUM(C57:C57)</f>
         <v>25</v>
       </c>
-      <c r="D58" s="21">
+      <c r="D58" s="22">
         <f>SUM(D57:D57)</f>
         <v>72</v>
       </c>
@@ -2233,14 +2974,14 @@
         <f>SUM(C57:E57)</f>
         <v>110</v>
       </c>
-      <c r="I58" s="22"/>
+      <c r="I58" s="23"/>
       <c r="K58" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M58" s="21">
+      <c r="M58" s="22">
         <v>60</v>
       </c>
       <c r="N58" s="6">
@@ -2255,12 +2996,12 @@
       </c>
     </row>
     <row r="59" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I59" s="22"/>
+      <c r="I59" s="23"/>
       <c r="K59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L59" s="5"/>
-      <c r="M59" s="21">
+      <c r="M59" s="22">
         <f>SUM(M57:M58)</f>
         <v>67</v>
       </c>
@@ -2278,36 +3019,36 @@
       </c>
     </row>
     <row r="60" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="22"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
+      <c r="P60" s="23"/>
     </row>
     <row r="61" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="I61" s="22"/>
-      <c r="K61" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L61" s="20"/>
-      <c r="M61" s="20"/>
-      <c r="N61" s="20"/>
-      <c r="O61" s="20"/>
-      <c r="P61" s="20"/>
+      <c r="A61" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" s="23"/>
+      <c r="K61" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
     </row>
     <row r="62" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -2319,7 +3060,7 @@
       <c r="C62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D62" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2328,7 +3069,7 @@
       <c r="F62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I62" s="22"/>
+      <c r="I62" s="23"/>
       <c r="K62" s="4" t="s">
         <v>0</v>
       </c>
@@ -2341,7 +3082,7 @@
       <c r="N62" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O62" s="27" t="s">
+      <c r="O62" s="29" t="s">
         <v>4</v>
       </c>
       <c r="P62" s="3" t="s">
@@ -2358,7 +3099,7 @@
       <c r="C63" s="6">
         <v>30</v>
       </c>
-      <c r="D63" s="21">
+      <c r="D63" s="22">
         <v>48</v>
       </c>
       <c r="E63" s="6">
@@ -2368,7 +3109,7 @@
         <f>SUM(C63:E63)</f>
         <v>95</v>
       </c>
-      <c r="I63" s="22"/>
+      <c r="I63" s="23"/>
       <c r="K63" s="4" t="s">
         <v>9</v>
       </c>
@@ -2381,7 +3122,7 @@
       <c r="N63" s="6">
         <v>7</v>
       </c>
-      <c r="O63" s="21">
+      <c r="O63" s="22">
         <v>19</v>
       </c>
       <c r="P63" s="7">
@@ -2398,7 +3139,7 @@
         <f>SUM(C63:C63)</f>
         <v>30</v>
       </c>
-      <c r="D64" s="21">
+      <c r="D64" s="22">
         <f>SUM(D63:D63)</f>
         <v>48</v>
       </c>
@@ -2410,7 +3151,7 @@
         <f>SUM(C63:E63)</f>
         <v>95</v>
       </c>
-      <c r="I64" s="22"/>
+      <c r="I64" s="23"/>
       <c r="K64" s="4" t="s">
         <v>10</v>
       </c>
@@ -2423,7 +3164,7 @@
       <c r="N64" s="6">
         <v>10</v>
       </c>
-      <c r="O64" s="21">
+      <c r="O64" s="22">
         <v>34</v>
       </c>
       <c r="P64" s="7">
@@ -2432,7 +3173,7 @@
       </c>
     </row>
     <row r="65" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I65" s="22"/>
+      <c r="I65" s="23"/>
       <c r="K65" s="4" t="s">
         <v>11</v>
       </c>
@@ -2445,7 +3186,7 @@
         <f>SUM(N63:N64)</f>
         <v>17</v>
       </c>
-      <c r="O65" s="21">
+      <c r="O65" s="22">
         <f>SUM(O63:O64)</f>
         <v>53</v>
       </c>
@@ -2455,42 +3196,42 @@
       </c>
     </row>
     <row r="66" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I66" s="22"/>
+      <c r="I66" s="23"/>
     </row>
     <row r="67" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="31"/>
-      <c r="J67" s="31"/>
-      <c r="K67" s="31"/>
-      <c r="L67" s="31"/>
-      <c r="M67" s="31"/>
-      <c r="N67" s="31"/>
-      <c r="O67" s="31"/>
-      <c r="P67" s="32"/>
+      <c r="A67" s="32"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="34"/>
     </row>
     <row r="68" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="29" t="s">
-        <v>44</v>
+      <c r="A68" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
@@ -2498,7 +3239,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
@@ -2506,7 +3247,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
@@ -2514,7 +3255,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
@@ -2522,7 +3263,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
@@ -2530,21 +3271,1732 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="6">
+        <v>30</v>
+      </c>
+      <c r="D81" s="6">
+        <v>48</v>
+      </c>
+      <c r="E81" s="6">
+        <v>17</v>
+      </c>
+      <c r="F81" s="7">
+        <f>SUM(C81:E81)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="6">
+        <v>25</v>
+      </c>
+      <c r="D82" s="6">
+        <v>72</v>
+      </c>
+      <c r="E82" s="6">
+        <v>13</v>
+      </c>
+      <c r="F82" s="7">
+        <f t="shared" ref="F82:F86" si="13">SUM(C82:E82)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="6">
+        <v>7</v>
+      </c>
+      <c r="D83" s="6">
+        <v>0</v>
+      </c>
+      <c r="E83" s="6">
+        <v>5</v>
+      </c>
+      <c r="F83" s="7">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="6">
+        <v>8</v>
+      </c>
+      <c r="D84" s="6">
+        <v>7</v>
+      </c>
+      <c r="E84" s="6">
+        <v>19</v>
+      </c>
+      <c r="F84" s="7">
+        <f t="shared" si="13"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="6">
+        <v>60</v>
+      </c>
+      <c r="D85" s="6">
+        <v>2</v>
+      </c>
+      <c r="E85" s="6">
+        <v>17</v>
+      </c>
+      <c r="F85" s="7">
+        <f t="shared" si="13"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="6">
+        <v>26</v>
+      </c>
+      <c r="D86" s="6">
+        <v>10</v>
+      </c>
+      <c r="E86" s="6">
+        <v>34</v>
+      </c>
+      <c r="F86" s="7">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="7">
+        <f>SUM(C81:C86)</f>
+        <v>156</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" ref="D87:E87" si="14">SUM(D81:D86)</f>
+        <v>139</v>
+      </c>
+      <c r="E87" s="7">
+        <f t="shared" si="14"/>
+        <v>105</v>
+      </c>
+      <c r="F87" s="7">
+        <f>SUM(C81:E86)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91">
+        <f>C87</f>
+        <v>156</v>
+      </c>
+      <c r="C91">
+        <f>Table29[[#This Row],[Count]]/$F$87</f>
+        <v>0.39</v>
+      </c>
+      <c r="D91">
+        <f>LOG(Table29[[#This Row],[Proportion]], 2)</f>
+        <v>-1.3584539709124763</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <f>D87</f>
+        <v>139</v>
+      </c>
+      <c r="C92">
+        <f>Table29[[#This Row],[Count]]/$F$87</f>
+        <v>0.34749999999999998</v>
+      </c>
+      <c r="D92">
+        <f>LOG(Table29[[#This Row],[Proportion]], 2)</f>
+        <v>-1.5249151170512174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93">
+        <f>E87</f>
+        <v>105</v>
+      </c>
+      <c r="C93">
+        <f>Table29[[#This Row],[Count]]/$F$87</f>
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="D93">
+        <f>LOG(Table29[[#This Row],[Proportion]], 2)</f>
+        <v>-1.9296106721086022</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B95" s="13" cm="1">
+        <f t="array" ref="B95">-SUM(Table29[Proportion] * Table29[log2(Proportion)])</f>
+        <v>1.5662278532596718</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A97" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+      <c r="C97" t="s">
+        <v>50</v>
+      </c>
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" t="s">
+        <v>52</v>
+      </c>
+      <c r="F97" t="s">
+        <v>53</v>
+      </c>
+      <c r="G97" t="s">
+        <v>54</v>
+      </c>
+      <c r="H97" t="s">
+        <v>58</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J97" t="s">
+        <v>57</v>
+      </c>
+      <c r="K97" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A98" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98">
+        <f>(C81+C82) / $F$87</f>
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="C98">
+        <f>(D81+D82) / $F$87</f>
+        <v>0.3</v>
+      </c>
+      <c r="D98">
+        <f>(E81+E82) / $F$87</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E98">
+        <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-2.8624964762500649</v>
+      </c>
+      <c r="F98">
+        <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-1.7369655941662063</v>
+      </c>
+      <c r="G98">
+        <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-3.7369655941662066</v>
+      </c>
+      <c r="H98">
+        <f>F81+F82</f>
+        <v>205</v>
+      </c>
+      <c r="I98" s="14" cm="1">
+        <f t="array" ref="I98">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
+        <v>1.1949553632967114</v>
+      </c>
+      <c r="J98" s="14" cm="1">
+        <f t="array" ref="J98">-SUM(B99:D100*E99:G100)</f>
+        <v>1.5307150056166299</v>
+      </c>
+      <c r="K98">
+        <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
+        <v>0.2075896643320001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A99" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99">
+        <f>(C83+C84) / $F$87</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="C99">
+        <f t="shared" ref="C99:D99" si="15">(D83+D84) / $F$87</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="15"/>
+        <v>0.06</v>
+      </c>
+      <c r="E99">
+        <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-4.7369655941662066</v>
+      </c>
+      <c r="F99">
+        <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-5.8365012677171197</v>
+      </c>
+      <c r="G99">
+        <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-4.0588936890535683</v>
+      </c>
+      <c r="H99">
+        <f>F83+F84</f>
+        <v>46</v>
+      </c>
+      <c r="I99" s="14" cm="1">
+        <f t="array" ref="I99">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
+        <v>0.52330860330949647</v>
+      </c>
+      <c r="J99" s="14" cm="1">
+        <f t="array" ref="J99">-SUM(B98:D98*E98:G98) -SUM(B100:D100*E100:G100)</f>
+        <v>2.202361765603845</v>
+      </c>
+      <c r="K99">
+        <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
+        <v>-0.44304279868032292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A100" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100">
+        <f>(C85+C86) / $F$87</f>
+        <v>0.215</v>
+      </c>
+      <c r="C100">
+        <f t="shared" ref="C100:D100" si="16">(D85+D86) / $F$87</f>
+        <v>0.03</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="16"/>
+        <v>0.1275</v>
+      </c>
+      <c r="E100">
+        <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-2.2175914350726269</v>
+      </c>
+      <c r="F100">
+        <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-5.0588936890535692</v>
+      </c>
+      <c r="G100">
+        <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-2.9714308478032287</v>
+      </c>
+      <c r="H100">
+        <f>F85+F86</f>
+        <v>149</v>
+      </c>
+      <c r="I100" s="14" cm="1">
+        <f t="array" ref="I100">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
+        <v>1.0074064023071336</v>
+      </c>
+      <c r="J100" s="14" cm="1">
+        <f t="array" ref="J100">-SUM(B98:D99*E98:G99)</f>
+        <v>1.7182639666062078</v>
+      </c>
+      <c r="K100">
+        <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
+        <v>0.11275832935486907</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A101" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="39">
+        <f>(C81+C83+C85) / $F$87</f>
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="C101" s="39">
+        <f t="shared" ref="C101:D101" si="17">(D81+D83+D85) / $F$87</f>
+        <v>0.125</v>
+      </c>
+      <c r="D101" s="39">
+        <f t="shared" si="17"/>
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="E101" s="39">
+        <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-2.043943347587597</v>
+      </c>
+      <c r="F101" s="39">
+        <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-3</v>
+      </c>
+      <c r="G101" s="39">
+        <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-3.3584539709124761</v>
+      </c>
+      <c r="H101" s="39">
+        <f>F81+F83+F85</f>
+        <v>186</v>
+      </c>
+      <c r="I101" s="40" cm="1">
+        <f t="array" ref="I101">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
+        <v>1.1981055239539586</v>
+      </c>
+      <c r="J101" s="40" cm="1">
+        <f t="array" ref="J101">-SUM(B102:D102 * E102:G102)</f>
+        <v>1.3185974936644378</v>
+      </c>
+      <c r="K101" s="39">
+        <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
+        <v>0.3036591255106067</v>
+      </c>
+      <c r="L101" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A102" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <f>(C82+C84+C86) / $F$87</f>
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="C102">
+        <f t="shared" ref="C102:D102" si="18">(D82+D84+D86) / $F$87</f>
+        <v>0.2225</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="18"/>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E102">
+        <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-2.7612131404128837</v>
+      </c>
+      <c r="F102">
+        <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-2.1681227588083267</v>
+      </c>
+      <c r="G102">
+        <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-2.599462070416271</v>
+      </c>
+      <c r="H102">
+        <f>F82+F84+F86</f>
+        <v>214</v>
+      </c>
+      <c r="I102" s="14" cm="1">
+        <f t="array" ref="I102">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
+        <v>1.3185974936644378</v>
+      </c>
+      <c r="J102" s="14" cm="1">
+        <f t="array" ref="J102">-SUM(B101:D101 * E101:G101)</f>
+        <v>1.1981055239539586</v>
+      </c>
+      <c r="K102">
+        <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
+        <v>0.3036591255106067</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="32"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="33"/>
+      <c r="F105" s="33"/>
+      <c r="G105" s="33"/>
+      <c r="H105" s="33"/>
+      <c r="I105" s="35" t="s">
         <v>42</v>
+      </c>
+      <c r="J105" s="33"/>
+      <c r="K105" s="33"/>
+      <c r="L105" s="33"/>
+      <c r="M105" s="33"/>
+      <c r="N105" s="33"/>
+      <c r="O105" s="33"/>
+      <c r="P105" s="34"/>
+    </row>
+    <row r="106" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I106" s="23"/>
+      <c r="K106" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10"/>
+      <c r="O106" s="10"/>
+      <c r="P106" s="10"/>
+    </row>
+    <row r="107" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I107" s="23"/>
+      <c r="K107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N107" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O107" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="6">
+        <v>30</v>
+      </c>
+      <c r="D108" s="6">
+        <v>48</v>
+      </c>
+      <c r="E108" s="6">
+        <v>17</v>
+      </c>
+      <c r="F108" s="7">
+        <f>SUM(C108:E108)</f>
+        <v>95</v>
+      </c>
+      <c r="I108" s="23"/>
+      <c r="K108" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M108" s="6">
+        <v>25</v>
+      </c>
+      <c r="N108" s="6">
+        <v>72</v>
+      </c>
+      <c r="O108" s="6">
+        <v>13</v>
+      </c>
+      <c r="P108" s="7">
+        <f t="shared" ref="P108:P110" si="19">SUM(M108:O108)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="6">
+        <v>7</v>
+      </c>
+      <c r="D109" s="6">
+        <v>0</v>
+      </c>
+      <c r="E109" s="6">
+        <v>5</v>
+      </c>
+      <c r="F109" s="7">
+        <f t="shared" ref="F109:F110" si="20">SUM(C109:E109)</f>
+        <v>12</v>
+      </c>
+      <c r="I109" s="23"/>
+      <c r="K109" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M109" s="6">
+        <v>8</v>
+      </c>
+      <c r="N109" s="6">
+        <v>7</v>
+      </c>
+      <c r="O109" s="6">
+        <v>19</v>
+      </c>
+      <c r="P109" s="7">
+        <f t="shared" si="19"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="6">
+        <v>60</v>
+      </c>
+      <c r="D110" s="6">
+        <v>2</v>
+      </c>
+      <c r="E110" s="6">
+        <v>17</v>
+      </c>
+      <c r="F110" s="7">
+        <f t="shared" si="20"/>
+        <v>79</v>
+      </c>
+      <c r="I110" s="23"/>
+      <c r="K110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M110" s="6">
+        <v>26</v>
+      </c>
+      <c r="N110" s="6">
+        <v>10</v>
+      </c>
+      <c r="O110" s="6">
+        <v>34</v>
+      </c>
+      <c r="P110" s="7">
+        <f t="shared" si="19"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" s="5"/>
+      <c r="C111" s="7">
+        <f>SUM(C108:C110)</f>
+        <v>97</v>
+      </c>
+      <c r="D111" s="7">
+        <f>SUM(D108:D110)</f>
+        <v>50</v>
+      </c>
+      <c r="E111" s="7">
+        <f>SUM(E108:E110)</f>
+        <v>39</v>
+      </c>
+      <c r="F111" s="7">
+        <f>SUM(C108:E110)</f>
+        <v>186</v>
+      </c>
+      <c r="I111" s="23"/>
+      <c r="K111" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L111" s="5"/>
+      <c r="M111" s="7">
+        <f>SUM(M108:M110)</f>
+        <v>59</v>
+      </c>
+      <c r="N111" s="7">
+        <f>SUM(N108:N110)</f>
+        <v>89</v>
+      </c>
+      <c r="O111" s="7">
+        <f>SUM(O108:O110)</f>
+        <v>66</v>
+      </c>
+      <c r="P111" s="7">
+        <f>SUM(M108:O110)</f>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I112" s="23"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I113" s="23"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" t="s">
+        <v>48</v>
+      </c>
+      <c r="I114" s="23"/>
+      <c r="K114" t="s">
+        <v>26</v>
+      </c>
+      <c r="L114" t="s">
+        <v>25</v>
+      </c>
+      <c r="M114" t="s">
+        <v>16</v>
+      </c>
+      <c r="N114" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115">
+        <f>C111</f>
+        <v>97</v>
+      </c>
+      <c r="C115">
+        <f>Table2934[[#This Row],[Count]]/$F$111</f>
+        <v>0.521505376344086</v>
+      </c>
+      <c r="D115">
+        <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
+        <v>-0.93924596892090373</v>
+      </c>
+      <c r="I115" s="23"/>
+      <c r="K115" t="s">
+        <v>2</v>
+      </c>
+      <c r="L115">
+        <f>M111</f>
+        <v>59</v>
+      </c>
+      <c r="M115">
+        <f>Table293437[[#This Row],[Count]]/$P$111</f>
+        <v>0.27570093457943923</v>
+      </c>
+      <c r="N115">
+        <f>LOG(Table293437[[#This Row],[Proportion]], 2)</f>
+        <v>-1.8588239370393058</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <f>D111</f>
+        <v>50</v>
+      </c>
+      <c r="C116">
+        <f>Table2934[[#This Row],[Count]]/$F$111</f>
+        <v>0.26881720430107525</v>
+      </c>
+      <c r="D116">
+        <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
+        <v>-1.8953026213333068</v>
+      </c>
+      <c r="I116" s="23"/>
+      <c r="K116" t="s">
+        <v>3</v>
+      </c>
+      <c r="L116">
+        <f>N111</f>
+        <v>89</v>
+      </c>
+      <c r="M116">
+        <f>Table293437[[#This Row],[Count]]/$P$111</f>
+        <v>0.41588785046728971</v>
+      </c>
+      <c r="N116">
+        <f>LOG(Table293437[[#This Row],[Proportion]], 2)</f>
+        <v>-1.2657335554347493</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117">
+        <f>E111</f>
+        <v>39</v>
+      </c>
+      <c r="C117">
+        <f>Table2934[[#This Row],[Count]]/$F$111</f>
+        <v>0.20967741935483872</v>
+      </c>
+      <c r="D117">
+        <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
+        <v>-2.2537565922457832</v>
+      </c>
+      <c r="I117" s="23"/>
+      <c r="K117" t="s">
+        <v>4</v>
+      </c>
+      <c r="L117">
+        <f>O111</f>
+        <v>66</v>
+      </c>
+      <c r="M117">
+        <f>Table293437[[#This Row],[Count]]/$P$111</f>
+        <v>0.30841121495327101</v>
+      </c>
+      <c r="N117">
+        <f>LOG(Table293437[[#This Row],[Proportion]], 2)</f>
+        <v>-1.6970728670426936</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I118" s="23"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A119" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B119" s="13" cm="1">
+        <f t="array" ref="B119">-SUM(Table2934[Proportion] * Table2934[log2(Proportion)])</f>
+        <v>1.4718736405891319</v>
+      </c>
+      <c r="I119" s="23"/>
+      <c r="K119" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L119" s="13" cm="1">
+        <f t="array" ref="L119">-SUM(Table293437[Proportion] * Table293437[log2(Proportion)])</f>
+        <v>1.5622790090833154</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I120" s="23"/>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A121" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B121" t="s">
+        <v>49</v>
+      </c>
+      <c r="C121" t="s">
+        <v>50</v>
+      </c>
+      <c r="D121" t="s">
+        <v>51</v>
+      </c>
+      <c r="E121" t="s">
+        <v>52</v>
+      </c>
+      <c r="F121" t="s">
+        <v>53</v>
+      </c>
+      <c r="G121" t="s">
+        <v>54</v>
+      </c>
+      <c r="H121" t="s">
+        <v>58</v>
+      </c>
+      <c r="I121" s="23"/>
+      <c r="K121" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="L121" t="s">
+        <v>49</v>
+      </c>
+      <c r="M121" t="s">
+        <v>50</v>
+      </c>
+      <c r="N121" t="s">
+        <v>51</v>
+      </c>
+      <c r="O121" t="s">
+        <v>52</v>
+      </c>
+      <c r="P121" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>54</v>
+      </c>
+      <c r="R121" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A122" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B122">
+        <f>C108/$F$111</f>
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="C122">
+        <f t="shared" ref="C122:D122" si="21">D108/$F$111</f>
+        <v>0.25806451612903225</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="21"/>
+        <v>9.1397849462365593E-2</v>
+      </c>
+      <c r="E122">
+        <f>LOG(Table3035[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-2.6322682154995132</v>
+      </c>
+      <c r="F122">
+        <f>LOG(Table3035[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-1.9541963103868754</v>
+      </c>
+      <c r="G122">
+        <f>LOG(Table3035[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-3.4516959698576919</v>
+      </c>
+      <c r="H122">
+        <f>F108</f>
+        <v>95</v>
+      </c>
+      <c r="I122" s="23"/>
+      <c r="K122" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="L122">
+        <f>M108/$P$111</f>
+        <v>0.11682242990654206</v>
+      </c>
+      <c r="M122">
+        <f t="shared" ref="M122:N122" si="22">N108/$P$111</f>
+        <v>0.3364485981308411</v>
+      </c>
+      <c r="N122">
+        <f t="shared" si="22"/>
+        <v>6.0747663551401869E-2</v>
+      </c>
+      <c r="O122">
+        <f>LOG(Table303538[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-3.0976107966264221</v>
+      </c>
+      <c r="P122">
+        <f>LOG(Table303538[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-1.5715419849588348</v>
+      </c>
+      <c r="Q122">
+        <f>LOG(Table303538[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-4.0410272682600548</v>
+      </c>
+      <c r="R122">
+        <f>P108</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A123" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123">
+        <f>C109/$F$111</f>
+        <v>3.7634408602150539E-2</v>
+      </c>
+      <c r="C123">
+        <f t="shared" ref="C123:D123" si="23">D109/$F$111</f>
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="23"/>
+        <v>2.6881720430107527E-2</v>
+      </c>
+      <c r="E123">
+        <f>LOG(Table3035[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-4.7318038890504273</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <f>LOG(Table3035[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-5.2172307162206693</v>
+      </c>
+      <c r="H123">
+        <f t="shared" ref="H123:H124" si="24">F109</f>
+        <v>12</v>
+      </c>
+      <c r="I123" s="23"/>
+      <c r="K123" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="L123">
+        <f t="shared" ref="L123:N123" si="25">M109/$P$111</f>
+        <v>3.7383177570093455E-2</v>
+      </c>
+      <c r="M123">
+        <f t="shared" si="25"/>
+        <v>3.2710280373831772E-2</v>
+      </c>
+      <c r="N123">
+        <f t="shared" si="25"/>
+        <v>8.8785046728971959E-2</v>
+      </c>
+      <c r="O123">
+        <f>LOG(Table303538[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-4.7414669864011465</v>
+      </c>
+      <c r="P123">
+        <v>0</v>
+      </c>
+      <c r="Q123">
+        <f>LOG(Table303538[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-3.4935394729575613</v>
+      </c>
+      <c r="R123">
+        <f t="shared" ref="R123:R124" si="26">P109</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A124" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B124">
+        <f>C110/$F$111</f>
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="C124">
+        <f t="shared" ref="C124:D124" si="27">D110/$F$111</f>
+        <v>1.0752688172043012E-2</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="27"/>
+        <v>9.1397849462365593E-2</v>
+      </c>
+      <c r="E124">
+        <f>LOG(Table3035[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-1.632268215499513</v>
+      </c>
+      <c r="F124">
+        <f>LOG(Table3035[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-6.5391588111080319</v>
+      </c>
+      <c r="G124">
+        <f>LOG(Table3035[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-3.4516959698576919</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="24"/>
+        <v>79</v>
+      </c>
+      <c r="I124" s="23"/>
+      <c r="K124" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="L124">
+        <f t="shared" ref="L124:N124" si="28">M110/$P$111</f>
+        <v>0.12149532710280374</v>
+      </c>
+      <c r="M124">
+        <f t="shared" si="28"/>
+        <v>4.6728971962616821E-2</v>
+      </c>
+      <c r="N124">
+        <f t="shared" si="28"/>
+        <v>0.15887850467289719</v>
+      </c>
+      <c r="O124">
+        <f>LOG(Table303538[[#This Row],[Proportion-Alcohol]], 2)</f>
+        <v>-3.0410272682600548</v>
+      </c>
+      <c r="P124">
+        <f>LOG(Table303538[[#This Row],[Proportion-Cocaine]], 2)</f>
+        <v>-4.4195388915137848</v>
+      </c>
+      <c r="Q124">
+        <f>LOG(Table303538[[#This Row],[Proportion-Heroin]], 2)</f>
+        <v>-2.6540041451508074</v>
+      </c>
+      <c r="R124">
+        <f t="shared" si="26"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I125" s="23"/>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A126" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B126" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C126" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D126" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="I126" s="23"/>
+      <c r="K126" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L126" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="M126" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="N126" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A127" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="50" cm="1">
+        <f t="array" ref="B127">-SUM(B122:D122*E122:G122)</f>
+        <v>1.2443457035007321</v>
+      </c>
+      <c r="C127" s="50" cm="1">
+        <f t="array" ref="C127">-SUM(B123:D124*E123:G124)</f>
+        <v>1.2306560367969031</v>
+      </c>
+      <c r="D127" s="51">
+        <f>$B$119 - ((H122/$F$111) * B127 + (($F$111-H122)/$F$111) * C127)</f>
+        <v>0.23422556972306885</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I127" s="23"/>
+      <c r="K127" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="L127" s="53" cm="1">
+        <f t="array" ref="L127">-SUM(L122:N122*O122:Q122)</f>
+        <v>1.1360964828040998</v>
+      </c>
+      <c r="M127" s="53" cm="1">
+        <f t="array" ref="M127">-SUM(L123:N124*O123:Q124)</f>
+        <v>1.4850804892636895</v>
+      </c>
+      <c r="N127" s="54">
+        <f>$L$119 - ((R122/$P$111) * L127 + (($P$111-R122)/$P$111) * M127)</f>
+        <v>0.2565828222053963</v>
+      </c>
+      <c r="O127" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A128" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128" s="47" cm="1">
+        <f t="array" ref="B128">-SUM(B123:D123*E123:G123)</f>
+        <v>0.31832677851858249</v>
+      </c>
+      <c r="C128" s="47" cm="1">
+        <f t="array" ref="C128">-SUM(B122:D122*E122:G122) -SUM(B124:D124*E124:G124)</f>
+        <v>2.1566749617790526</v>
+      </c>
+      <c r="D128" s="48">
+        <f t="shared" ref="D128:D129" si="29">$B$119 - ((H123/$F$111) * B128 + (($F$111-H123)/$F$111) * C128)</f>
+        <v>-0.56619821259247116</v>
+      </c>
+      <c r="I128" s="23"/>
+      <c r="K128" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="L128" s="47" cm="1">
+        <f t="array" ref="L128">-SUM(L123:N123*O123:Q123)</f>
+        <v>0.48742516765141508</v>
+      </c>
+      <c r="M128" s="47" cm="1">
+        <f t="array" ref="M128">-SUM(L122:N122*O122:Q122) -SUM(L124:N124*O124:Q124)</f>
+        <v>2.1337518044163741</v>
+      </c>
+      <c r="N128" s="48">
+        <f>$L$119 - ((R123/$P$111) * L128 + (($P$111-R123)/$P$111) * M128)</f>
+        <v>-0.30990688108068198</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A129" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" s="45" cm="1">
+        <f t="array" ref="B129">-SUM(B124:D124*E124:G124)</f>
+        <v>0.91232925827832045</v>
+      </c>
+      <c r="C129" s="45" cm="1">
+        <f t="array" ref="C129">-SUM(B122:D123*E122:G123)</f>
+        <v>1.5626724820193147</v>
+      </c>
+      <c r="D129" s="48">
+        <f t="shared" si="29"/>
+        <v>0.18542220521249742</v>
+      </c>
+      <c r="I129" s="23"/>
+      <c r="K129" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="L129" s="45" cm="1">
+        <f t="array" ref="L129">-SUM(L124:N124*O124:Q124)</f>
+        <v>0.99765532161227433</v>
+      </c>
+      <c r="M129" s="45" cm="1">
+        <f t="array" ref="M129">-SUM(L122:N123*O122:Q123)</f>
+        <v>1.623521650455515</v>
+      </c>
+      <c r="N129" s="11">
+        <f t="shared" ref="N129" si="30">$L$119 - ((R124/$P$111) * L129 + (($P$111-R124)/$P$111) * M129)</f>
+        <v>0.14347998955783248</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I130" s="23"/>
+    </row>
+    <row r="131" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I131" s="23"/>
+    </row>
+    <row r="132" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="23"/>
+      <c r="B132" s="23"/>
+      <c r="C132" s="23"/>
+      <c r="D132" s="23"/>
+      <c r="E132" s="23"/>
+      <c r="F132" s="23"/>
+      <c r="G132" s="23"/>
+      <c r="H132" s="23"/>
+      <c r="I132" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J132" s="23"/>
+      <c r="K132" s="23"/>
+      <c r="L132" s="23"/>
+      <c r="M132" s="23"/>
+      <c r="N132" s="23"/>
+      <c r="O132" s="23"/>
+      <c r="P132" s="23"/>
+      <c r="Q132" s="23"/>
+      <c r="R132" s="23"/>
+    </row>
+    <row r="133" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I133" s="23"/>
+    </row>
+    <row r="134" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I134" s="23"/>
+      <c r="K134" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L134" s="10"/>
+      <c r="M134" s="10"/>
+      <c r="N134" s="10"/>
+      <c r="O134" s="10"/>
+      <c r="P134" s="10"/>
+    </row>
+    <row r="135" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I135" s="23"/>
+      <c r="K135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M135" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N135" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O135" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P135" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="6">
+        <v>30</v>
+      </c>
+      <c r="D136" s="22">
+        <v>48</v>
+      </c>
+      <c r="E136" s="6">
+        <v>17</v>
+      </c>
+      <c r="F136" s="7">
+        <f>SUM(C136:E136)</f>
+        <v>95</v>
+      </c>
+      <c r="I136" s="23"/>
+      <c r="K136" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M136" s="6">
+        <v>25</v>
+      </c>
+      <c r="N136" s="22">
+        <v>72</v>
+      </c>
+      <c r="O136" s="6">
+        <v>13</v>
+      </c>
+      <c r="P136" s="7">
+        <f t="shared" ref="P136" si="31">SUM(M136:O136)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B137" s="5"/>
+      <c r="C137" s="7">
+        <f>SUM(C136:C136)</f>
+        <v>30</v>
+      </c>
+      <c r="D137" s="22">
+        <f>SUM(D136:D136)</f>
+        <v>48</v>
+      </c>
+      <c r="E137" s="7">
+        <f>SUM(E136:E136)</f>
+        <v>17</v>
+      </c>
+      <c r="F137" s="7">
+        <f>SUM(C136:E136)</f>
+        <v>95</v>
+      </c>
+      <c r="I137" s="23"/>
+      <c r="K137" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L137" s="5"/>
+      <c r="M137" s="7">
+        <f>SUM(M136:M136)</f>
+        <v>25</v>
+      </c>
+      <c r="N137" s="22">
+        <f>SUM(N136:N136)</f>
+        <v>72</v>
+      </c>
+      <c r="O137" s="7">
+        <f>SUM(O136:O136)</f>
+        <v>13</v>
+      </c>
+      <c r="P137" s="7">
+        <f>SUM(M136:O136)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I138" s="23"/>
+    </row>
+    <row r="139" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I139" s="23"/>
+      <c r="K139" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L139" s="10"/>
+      <c r="M139" s="10"/>
+      <c r="N139" s="10"/>
+      <c r="O139" s="10"/>
+      <c r="P139" s="10"/>
+    </row>
+    <row r="140" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I140" s="23"/>
+      <c r="K140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L140" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M140" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N140" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O140" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P140" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="22">
+        <v>7</v>
+      </c>
+      <c r="D141" s="6">
+        <v>0</v>
+      </c>
+      <c r="E141" s="6">
+        <v>5</v>
+      </c>
+      <c r="F141" s="7">
+        <f t="shared" ref="F141:F142" si="32">SUM(C141:E141)</f>
+        <v>12</v>
+      </c>
+      <c r="I141" s="23"/>
+      <c r="K141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M141" s="6">
+        <v>8</v>
+      </c>
+      <c r="N141" s="6">
+        <v>7</v>
+      </c>
+      <c r="O141" s="22">
+        <v>19</v>
+      </c>
+      <c r="P141" s="7">
+        <f t="shared" ref="P141:P142" si="33">SUM(M141:O141)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="22">
+        <v>60</v>
+      </c>
+      <c r="D142" s="6">
+        <v>2</v>
+      </c>
+      <c r="E142" s="6">
+        <v>17</v>
+      </c>
+      <c r="F142" s="7">
+        <f t="shared" si="32"/>
+        <v>79</v>
+      </c>
+      <c r="I142" s="23"/>
+      <c r="K142" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M142" s="6">
+        <v>26</v>
+      </c>
+      <c r="N142" s="6">
+        <v>10</v>
+      </c>
+      <c r="O142" s="22">
+        <v>34</v>
+      </c>
+      <c r="P142" s="7">
+        <f t="shared" si="33"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B143" s="5"/>
+      <c r="C143" s="22">
+        <f>SUM(C141:C142)</f>
+        <v>67</v>
+      </c>
+      <c r="D143" s="7">
+        <f>SUM(D141:D142)</f>
+        <v>2</v>
+      </c>
+      <c r="E143" s="7">
+        <f>SUM(E141:E142)</f>
+        <v>22</v>
+      </c>
+      <c r="F143" s="7">
+        <f>SUM(C141:E142)</f>
+        <v>91</v>
+      </c>
+      <c r="I143" s="23"/>
+      <c r="K143" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L143" s="5"/>
+      <c r="M143" s="7">
+        <f>SUM(M141:M142)</f>
+        <v>34</v>
+      </c>
+      <c r="N143" s="7">
+        <f>SUM(N141:N142)</f>
+        <v>17</v>
+      </c>
+      <c r="O143" s="22">
+        <f>SUM(O141:O142)</f>
+        <v>53</v>
+      </c>
+      <c r="P143" s="7">
+        <f>SUM(M141:O142)</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I144" s="23"/>
+    </row>
+    <row r="145" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I145" s="23"/>
+    </row>
+    <row r="146" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="32"/>
+      <c r="B146" s="33"/>
+      <c r="C146" s="33"/>
+      <c r="D146" s="33"/>
+      <c r="E146" s="33"/>
+      <c r="F146" s="33"/>
+      <c r="G146" s="33"/>
+      <c r="H146" s="33"/>
+      <c r="I146" s="33"/>
+      <c r="J146" s="33"/>
+      <c r="K146" s="33"/>
+      <c r="L146" s="33"/>
+      <c r="M146" s="33"/>
+      <c r="N146" s="33"/>
+      <c r="O146" s="33"/>
+      <c r="P146" s="34"/>
+    </row>
+    <row r="147" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>40</v>
+      </c>
+      <c r="B148" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>18</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>19</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>20</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>21</v>
+      </c>
+      <c r="B153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>22</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="7">
+  <tableParts count="16">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -2552,6 +5004,15 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final commit for final exam
</commit_message>
<xml_diff>
--- a/CS-513/FinalExam/final_problem1.xlsx
+++ b/CS-513/FinalExam/final_problem1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyatthenryblair/Desktop/Projects/Stevens/CS-513/FinalExam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4205589-2844-5B45-A4E2-760B9C98F47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72095251-7FC1-2E44-93AB-1B604C6CEB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="840" windowWidth="28040" windowHeight="17420" xr2:uid="{5CD4EC78-82A5-1D4F-B2C7-988FE798375A}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="70">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -243,7 +243,31 @@
     <t>&lt;-- Highest Information Gain is if we split on Black / not Black</t>
   </si>
   <si>
-    <t>--&gt; Identical to 1.a)</t>
+    <t>--&gt; Identical to 1.a), just got there with a different ordering of the splits</t>
+  </si>
+  <si>
+    <t>Black-Young --&gt; Cocaine</t>
+  </si>
+  <si>
+    <t>Black-Old --&gt; Cocaine</t>
+  </si>
+  <si>
+    <t>Hispanic-Old --&gt; Alcohol</t>
+  </si>
+  <si>
+    <t>White-Old--&gt; Alcohol</t>
+  </si>
+  <si>
+    <t>Hispanic-Young --&gt; Heroin</t>
+  </si>
+  <si>
+    <t>White-Young --&gt; Heroin</t>
+  </si>
+  <si>
+    <t>White-Old --&gt; Alcohol</t>
+  </si>
+  <si>
+    <t>Hispanic-Old  --&gt; Alcohol</t>
   </si>
 </sst>
 </file>
@@ -387,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +480,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -673,7 +703,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -698,32 +728,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -740,18 +765,20 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
@@ -843,13 +870,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="1"/>
         </left>
@@ -859,6 +879,13 @@
         <top style="thin">
           <color theme="1"/>
         </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
@@ -899,30 +926,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1007,13 +1010,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="1"/>
         </left>
@@ -1027,6 +1023,37 @@
           <color theme="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1189,15 +1216,15 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{D5953D6F-FB9F-264F-AC79-0695F35359AD}" name="Table35" displayName="Table35" ref="A126:D129" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{D5953D6F-FB9F-264F-AC79-0695F35359AD}" name="Table35" displayName="Table35" ref="A126:D129" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A126:D129" xr:uid="{D5953D6F-FB9F-264F-AC79-0695F35359AD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8D16C576-2D75-A54C-8427-4BE82FC6F7DD}" name="Possible Split"/>
-    <tableColumn id="2" xr3:uid="{8A308947-5145-A042-96C6-12D3867C7CF6}" name="Entropy-LEFT" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{8A308947-5145-A042-96C6-12D3867C7CF6}" name="Entropy-LEFT" dataDxfId="8">
       <calculatedColumnFormula array="1">-SUM(B122:D122*E122:G122)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{44A464E1-0A52-F149-8F96-FA1A7ECD8993}" name="Entropy-RIGHT"/>
-    <tableColumn id="4" xr3:uid="{4855F0AF-3A2B-9E45-821C-63A25EAD374F}" name="Information Gain" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{4855F0AF-3A2B-9E45-821C-63A25EAD374F}" name="Information Gain" dataDxfId="7">
       <calculatedColumnFormula>$B$119 - ((H122/$F$111) * B127 + (($F$111-H122)/$F$111) * C127)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1256,7 +1283,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{6F100573-32FC-7E4E-BC13-4C639F7894F7}" name="Table3539" displayName="Table3539" ref="K126:N129" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{6F100573-32FC-7E4E-BC13-4C639F7894F7}" name="Table3539" displayName="Table3539" ref="K126:N129" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="K126:N129" xr:uid="{6F100573-32FC-7E4E-BC13-4C639F7894F7}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C02457B7-66AA-EA42-8451-1EFFF213F3DB}" name="Possible Split"/>
@@ -1741,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E81D6DC-F462-584B-94C4-8AECFCC18FE7}">
   <dimension ref="A1:S154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="J47" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1774,40 +1801,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="M1" s="9"/>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1999,9 +2026,14 @@
       <c r="M14" s="9"/>
     </row>
     <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="51" t="s">
         <v>14</v>
       </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2039,10 +2071,10 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <f>1 - (B19^2 + B20^2 + B21^2)</f>
         <v>0.65823750000000003</v>
       </c>
@@ -2074,34 +2106,34 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="14">
         <f>C6+C7</f>
         <v>55</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <f>D6+D7</f>
         <v>120</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="14">
         <f>E6+E7</f>
         <v>30</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="14">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.26829268292682928</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="14">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.58536585365853655</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="14">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.14634146341463414</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="15">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.56395002974419994</v>
       </c>
@@ -2125,19 +2157,19 @@
         <f>E8+E9</f>
         <v>24</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32608695652173914</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.15217391304347827</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.59829867674858228</v>
       </c>
@@ -2158,19 +2190,19 @@
         <f>E10+E11</f>
         <v>51</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.57718120805369133</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>8.0536912751677847E-2</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.34228187919463088</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.54321877392910223</v>
       </c>
@@ -2180,30 +2212,30 @@
         <v>7</v>
       </c>
       <c r="B29">
-        <f>C6+C8+C10</f>
+        <f t="shared" ref="B29:D30" si="2">C6+C8+C10</f>
         <v>97</v>
       </c>
       <c r="C29">
-        <f>D6+D8+D10</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="D29">
-        <f>E6+E8+E10</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.521505376344086</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.26881720430107525</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.20967741935483872</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="13">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.61180483292866228</v>
       </c>
@@ -2213,71 +2245,63 @@
         <v>8</v>
       </c>
       <c r="B30">
-        <f>C7+C9+C11</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="C30">
-        <f>D7+D9+D11</f>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="D30">
-        <f>E7+E9+E11</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30">
         <f>Table22[[#This Row],[Count-Alcohol]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.27570093457943923</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30">
         <f>Table22[[#This Row],[Count-Cocaine]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.41588785046728971</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30">
         <f>Table22[[#This Row],[Count-Heroin]]/SUM(Table22[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.30841121495327101</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <f>1 - SUMSQ(Table22[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.65590881299676829</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="15"/>
-      <c r="H31" s="15"/>
-    </row>
+    <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="35" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="34"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="29"/>
     </row>
     <row r="33" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I33" s="23"/>
-      <c r="K33" s="31" t="s">
+      <c r="I33" s="19"/>
+      <c r="K33" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -2298,7 +2322,7 @@
       <c r="F34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="23"/>
+      <c r="I34" s="19"/>
       <c r="K34" s="4" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2362,7 @@
         <f>SUM(C35:E35)</f>
         <v>95</v>
       </c>
-      <c r="I35" s="23"/>
+      <c r="I35" s="19"/>
       <c r="K35" s="4" t="s">
         <v>9</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>5</v>
       </c>
       <c r="P35" s="7">
-        <f t="shared" ref="P35:P38" si="2">SUM(M35:O35)</f>
+        <f t="shared" ref="P35:P38" si="3">SUM(M35:O35)</f>
         <v>12</v>
       </c>
     </row>
@@ -2374,10 +2398,10 @@
         <v>13</v>
       </c>
       <c r="F36" s="7">
-        <f t="shared" ref="F36" si="3">SUM(C36:E36)</f>
+        <f t="shared" ref="F36" si="4">SUM(C36:E36)</f>
         <v>110</v>
       </c>
-      <c r="I36" s="23"/>
+      <c r="I36" s="19"/>
       <c r="K36" s="4"/>
       <c r="L36" s="5" t="s">
         <v>8</v>
@@ -2392,7 +2416,7 @@
         <v>19</v>
       </c>
       <c r="P36" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
     </row>
@@ -2417,7 +2441,7 @@
         <f>SUM(C35:E36)</f>
         <v>205</v>
       </c>
-      <c r="I37" s="23"/>
+      <c r="I37" s="19"/>
       <c r="K37" s="4" t="s">
         <v>10</v>
       </c>
@@ -2434,12 +2458,12 @@
         <v>17</v>
       </c>
       <c r="P37" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="23"/>
+      <c r="I38" s="19"/>
       <c r="K38" s="4"/>
       <c r="L38" s="5" t="s">
         <v>8</v>
@@ -2454,12 +2478,12 @@
         <v>34</v>
       </c>
       <c r="P38" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="23"/>
+      <c r="I39" s="19"/>
       <c r="K39" s="4" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2506,7 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I40" s="23"/>
+      <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -2491,7 +2515,7 @@
       <c r="B41" t="s">
         <v>27</v>
       </c>
-      <c r="I41" s="23"/>
+      <c r="I41" s="19"/>
       <c r="K41" t="s">
         <v>26</v>
       </c>
@@ -2507,7 +2531,7 @@
         <f>$C$37/$F$37</f>
         <v>0.26829268292682928</v>
       </c>
-      <c r="I42" s="23"/>
+      <c r="I42" s="19"/>
       <c r="K42" t="s">
         <v>2</v>
       </c>
@@ -2524,7 +2548,7 @@
         <f>$D$37/$F$37</f>
         <v>0.58536585365853655</v>
       </c>
-      <c r="I43" s="23"/>
+      <c r="I43" s="19"/>
       <c r="K43" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2565,7 @@
         <f>$E$37/$F$37</f>
         <v>0.14634146341463414</v>
       </c>
-      <c r="I44" s="23"/>
+      <c r="I44" s="19"/>
       <c r="K44" t="s">
         <v>4</v>
       </c>
@@ -2551,27 +2575,27 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I45" s="23"/>
+      <c r="I45" s="19"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="12">
         <f>1 - SUMSQ(Table212426[P(Class)])</f>
         <v>0.56395002974419994</v>
       </c>
-      <c r="I46" s="23"/>
-      <c r="K46" s="12" t="s">
+      <c r="I46" s="19"/>
+      <c r="K46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L46" s="13">
+      <c r="L46" s="12">
         <f>1 - SUMSQ(Table2124[P(Class)])</f>
         <v>0.57430637738330037</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I47" s="30"/>
+      <c r="I47" s="25"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2598,7 +2622,7 @@
       <c r="H48" t="s">
         <v>24</v>
       </c>
-      <c r="I48" s="23"/>
+      <c r="I48" s="19"/>
       <c r="K48" t="s">
         <v>28</v>
       </c>
@@ -2633,30 +2657,30 @@
         <v>30</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:D49" si="4">D35</f>
+        <f t="shared" ref="C49:D49" si="5">D35</f>
         <v>48</v>
       </c>
       <c r="D49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49">
         <f>Table222527[[#This Row],[Count-Alcohol]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.31578947368421051</v>
       </c>
-      <c r="F49" s="15">
+      <c r="F49">
         <f>Table222527[[#This Row],[Count-Cocaine]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.50526315789473686</v>
       </c>
-      <c r="G49" s="15">
+      <c r="G49">
         <f>Table222527[[#This Row],[Count-Heroin]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.17894736842105263</v>
       </c>
-      <c r="H49" s="14">
+      <c r="H49" s="13">
         <f>1 - SUMSQ(Table222527[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.61296398891966764</v>
       </c>
-      <c r="I49" s="30"/>
+      <c r="I49" s="25"/>
       <c r="K49" t="s">
         <v>9</v>
       </c>
@@ -2665,64 +2689,64 @@
         <v>15</v>
       </c>
       <c r="M49">
-        <f t="shared" ref="M49:N49" si="5">N35+N36</f>
+        <f t="shared" ref="M49:N49" si="6">N35+N36</f>
         <v>7</v>
       </c>
       <c r="N49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="O49" s="15">
+      <c r="O49">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32608695652173914</v>
       </c>
-      <c r="P49" s="15">
+      <c r="P49">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.15217391304347827</v>
       </c>
-      <c r="Q49" s="15">
+      <c r="Q49">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="R49" s="14">
+      <c r="R49" s="13">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.59829867674858228</v>
       </c>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="14">
         <f>C36</f>
         <v>25</v>
       </c>
-      <c r="C50" s="16">
-        <f t="shared" ref="C50:D50" si="6">D36</f>
+      <c r="C50" s="14">
+        <f t="shared" ref="C50:D50" si="7">D36</f>
         <v>72</v>
       </c>
-      <c r="D50" s="16">
-        <f t="shared" si="6"/>
+      <c r="D50" s="14">
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="14">
         <f>Table222527[[#This Row],[Count-Alcohol]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.22727272727272727</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F50" s="14">
         <f>Table222527[[#This Row],[Count-Cocaine]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.65454545454545454</v>
       </c>
-      <c r="G50" s="17">
+      <c r="G50" s="14">
         <f>Table222527[[#This Row],[Count-Heroin]]/SUM(Table222527[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.11818181818181818</v>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="15">
         <f>1 - SUMSQ(Table222527[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.50595041322314049</v>
       </c>
-      <c r="I50" s="30" t="s">
+      <c r="I50" s="25" t="s">
         <v>39</v>
       </c>
       <c r="K50" t="s">
@@ -2733,60 +2757,60 @@
         <v>86</v>
       </c>
       <c r="M50">
-        <f t="shared" ref="M50:N50" si="7">N37+N38</f>
+        <f t="shared" ref="M50:N50" si="8">N37+N38</f>
         <v>12</v>
       </c>
       <c r="N50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>51</v>
       </c>
-      <c r="O50" s="15">
+      <c r="O50">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.57718120805369133</v>
       </c>
-      <c r="P50" s="15">
+      <c r="P50">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>8.0536912751677847E-2</v>
       </c>
-      <c r="Q50" s="15">
+      <c r="Q50">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.34228187919463088</v>
       </c>
-      <c r="R50" s="14">
+      <c r="R50" s="13">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.54321877392910223</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I51" s="23"/>
-      <c r="K51" s="16" t="s">
+      <c r="I51" s="19"/>
+      <c r="K51" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L51" s="16">
+      <c r="L51" s="14">
         <f>M35+M37</f>
         <v>67</v>
       </c>
-      <c r="M51" s="16">
-        <f t="shared" ref="M51:N51" si="8">N35+N37</f>
+      <c r="M51" s="14">
+        <f t="shared" ref="M51:N51" si="9">N35+N37</f>
         <v>2</v>
       </c>
-      <c r="N51" s="16">
-        <f t="shared" si="8"/>
+      <c r="N51" s="14">
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51" s="14">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.73626373626373631</v>
       </c>
-      <c r="P51" s="17">
+      <c r="P51" s="14">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>2.197802197802198E-2</v>
       </c>
-      <c r="Q51" s="17">
+      <c r="Q51" s="14">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.24175824175824176</v>
       </c>
-      <c r="R51" s="18">
+      <c r="R51" s="15">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.3989856297548604</v>
       </c>
@@ -2795,7 +2819,7 @@
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I52" s="23"/>
+      <c r="I52" s="19"/>
       <c r="K52" t="s">
         <v>8</v>
       </c>
@@ -2804,74 +2828,61 @@
         <v>34</v>
       </c>
       <c r="M52">
-        <f t="shared" ref="M52:N52" si="9">N36+N38</f>
+        <f t="shared" ref="M52:N52" si="10">N36+N38</f>
         <v>17</v>
       </c>
       <c r="N52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
-      <c r="O52" s="15">
+      <c r="O52">
         <f>Table2225[[#This Row],[Count-Alcohol]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.32692307692307693</v>
       </c>
-      <c r="P52" s="15">
+      <c r="P52">
         <f>Table2225[[#This Row],[Count-Cocaine]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.16346153846153846</v>
       </c>
-      <c r="Q52" s="15">
+      <c r="Q52">
         <f>Table2225[[#This Row],[Count-Heroin]]/SUM(Table2225[[#This Row],[Count-Alcohol]:[Count-Heroin]])</f>
         <v>0.50961538461538458</v>
       </c>
-      <c r="R52" s="14">
+      <c r="R52" s="13">
         <f>1 - SUMSQ(Table2225[[#This Row],[P(Alcohol | Split)]:[P(Heroin | Split)]])</f>
         <v>0.60669378698224852</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I53" s="23"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="32"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="36" t="s">
+      <c r="A54" s="27"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="34"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="28"/>
+      <c r="P54" s="29"/>
     </row>
     <row r="55" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="23"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="31" t="s">
+      <c r="I55" s="19"/>
+      <c r="K55" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
     </row>
     <row r="56" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
@@ -2883,7 +2894,7 @@
       <c r="C56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2892,14 +2903,14 @@
       <c r="F56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I56" s="23"/>
+      <c r="I56" s="19"/>
       <c r="K56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M56" s="29" t="s">
+      <c r="M56" s="24" t="s">
         <v>2</v>
       </c>
       <c r="N56" s="3" t="s">
@@ -2922,24 +2933,27 @@
       <c r="C57" s="6">
         <v>25</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="18">
         <v>72</v>
       </c>
       <c r="E57" s="6">
         <v>13</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" ref="F57" si="10">SUM(C57:E57)</f>
+        <f t="shared" ref="F57" si="11">SUM(C57:E57)</f>
         <v>110</v>
       </c>
-      <c r="I57" s="23"/>
+      <c r="G57" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I57" s="19"/>
       <c r="K57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M57" s="22">
+      <c r="M57" s="18">
         <v>7</v>
       </c>
       <c r="N57" s="6">
@@ -2949,8 +2963,11 @@
         <v>5</v>
       </c>
       <c r="P57" s="7">
-        <f t="shared" ref="P57:P58" si="11">SUM(M57:O57)</f>
+        <f t="shared" ref="P57:P58" si="12">SUM(M57:O57)</f>
         <v>12</v>
+      </c>
+      <c r="Q57" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -2962,7 +2979,7 @@
         <f>SUM(C57:C57)</f>
         <v>25</v>
       </c>
-      <c r="D58" s="22">
+      <c r="D58" s="18">
         <f>SUM(D57:D57)</f>
         <v>72</v>
       </c>
@@ -2974,14 +2991,14 @@
         <f>SUM(C57:E57)</f>
         <v>110</v>
       </c>
-      <c r="I58" s="23"/>
+      <c r="I58" s="19"/>
       <c r="K58" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M58" s="22">
+      <c r="M58" s="18">
         <v>60</v>
       </c>
       <c r="N58" s="6">
@@ -2991,17 +3008,20 @@
         <v>17</v>
       </c>
       <c r="P58" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>79</v>
       </c>
+      <c r="Q58" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="59" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I59" s="23"/>
+      <c r="I59" s="19"/>
       <c r="K59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L59" s="5"/>
-      <c r="M59" s="22">
+      <c r="M59" s="18">
         <f>SUM(M57:M58)</f>
         <v>67</v>
       </c>
@@ -3019,36 +3039,36 @@
       </c>
     </row>
     <row r="60" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
-      <c r="P60" s="23"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
+      <c r="N60" s="19"/>
+      <c r="O60" s="19"/>
+      <c r="P60" s="19"/>
     </row>
     <row r="61" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I61" s="23"/>
-      <c r="K61" s="25" t="s">
+      <c r="I61" s="19"/>
+      <c r="K61" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-      <c r="N61" s="21"/>
-      <c r="O61" s="21"/>
-      <c r="P61" s="21"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
     </row>
     <row r="62" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -3060,7 +3080,7 @@
       <c r="C62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="29" t="s">
+      <c r="D62" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -3069,7 +3089,7 @@
       <c r="F62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I62" s="23"/>
+      <c r="I62" s="19"/>
       <c r="K62" s="4" t="s">
         <v>0</v>
       </c>
@@ -3082,7 +3102,7 @@
       <c r="N62" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O62" s="29" t="s">
+      <c r="O62" s="24" t="s">
         <v>4</v>
       </c>
       <c r="P62" s="3" t="s">
@@ -3099,7 +3119,7 @@
       <c r="C63" s="6">
         <v>30</v>
       </c>
-      <c r="D63" s="22">
+      <c r="D63" s="18">
         <v>48</v>
       </c>
       <c r="E63" s="6">
@@ -3109,7 +3129,10 @@
         <f>SUM(C63:E63)</f>
         <v>95</v>
       </c>
-      <c r="I63" s="23"/>
+      <c r="G63" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I63" s="19"/>
       <c r="K63" s="4" t="s">
         <v>9</v>
       </c>
@@ -3122,12 +3145,15 @@
       <c r="N63" s="6">
         <v>7</v>
       </c>
-      <c r="O63" s="22">
+      <c r="O63" s="18">
         <v>19</v>
       </c>
       <c r="P63" s="7">
-        <f t="shared" ref="P63:P64" si="12">SUM(M63:O63)</f>
+        <f t="shared" ref="P63:P64" si="13">SUM(M63:O63)</f>
         <v>34</v>
+      </c>
+      <c r="Q63" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -3139,7 +3165,7 @@
         <f>SUM(C63:C63)</f>
         <v>30</v>
       </c>
-      <c r="D64" s="22">
+      <c r="D64" s="18">
         <f>SUM(D63:D63)</f>
         <v>48</v>
       </c>
@@ -3151,7 +3177,7 @@
         <f>SUM(C63:E63)</f>
         <v>95</v>
       </c>
-      <c r="I64" s="23"/>
+      <c r="I64" s="19"/>
       <c r="K64" s="4" t="s">
         <v>10</v>
       </c>
@@ -3164,16 +3190,19 @@
       <c r="N64" s="6">
         <v>10</v>
       </c>
-      <c r="O64" s="22">
+      <c r="O64" s="18">
         <v>34</v>
       </c>
       <c r="P64" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
+      <c r="Q64" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="65" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I65" s="23"/>
+      <c r="I65" s="19"/>
       <c r="K65" s="4" t="s">
         <v>11</v>
       </c>
@@ -3186,7 +3215,7 @@
         <f>SUM(N63:N64)</f>
         <v>17</v>
       </c>
-      <c r="O65" s="22">
+      <c r="O65" s="18">
         <f>SUM(O63:O64)</f>
         <v>53</v>
       </c>
@@ -3196,28 +3225,28 @@
       </c>
     </row>
     <row r="66" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I66" s="23"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
-      <c r="B67" s="33"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-      <c r="O67" s="33"/>
-      <c r="P67" s="34"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
+      <c r="K67" s="28"/>
+      <c r="L67" s="28"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="28"/>
+      <c r="P67" s="29"/>
     </row>
     <row r="68" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3278,9 +3307,14 @@
       </c>
     </row>
     <row r="78" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="51" t="s">
         <v>44</v>
       </c>
+      <c r="B78" s="52"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
+      <c r="E78" s="52"/>
+      <c r="F78" s="52"/>
     </row>
     <row r="79" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -3339,7 +3373,7 @@
         <v>13</v>
       </c>
       <c r="F82" s="7">
-        <f t="shared" ref="F82:F86" si="13">SUM(C82:E82)</f>
+        <f t="shared" ref="F82:F86" si="14">SUM(C82:E82)</f>
         <v>110</v>
       </c>
     </row>
@@ -3360,7 +3394,7 @@
         <v>5</v>
       </c>
       <c r="F83" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
     </row>
@@ -3379,7 +3413,7 @@
         <v>19</v>
       </c>
       <c r="F84" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>34</v>
       </c>
     </row>
@@ -3400,7 +3434,7 @@
         <v>17</v>
       </c>
       <c r="F85" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>79</v>
       </c>
     </row>
@@ -3419,7 +3453,7 @@
         <v>34</v>
       </c>
       <c r="F86" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>70</v>
       </c>
     </row>
@@ -3433,11 +3467,11 @@
         <v>156</v>
       </c>
       <c r="D87" s="7">
-        <f t="shared" ref="D87:E87" si="14">SUM(D81:D86)</f>
+        <f t="shared" ref="D87:E87" si="15">SUM(D81:D86)</f>
         <v>139</v>
       </c>
       <c r="E87" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>105</v>
       </c>
       <c r="F87" s="7">
@@ -3511,16 +3545,16 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B95" s="13" cm="1">
+      <c r="B95" s="12" cm="1">
         <f t="array" ref="B95">-SUM(Table29[Proportion] * Table29[log2(Proportion)])</f>
         <v>1.5662278532596718</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="37" t="s">
+      <c r="A97" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B97" t="s">
@@ -3544,7 +3578,7 @@
       <c r="H97" t="s">
         <v>58</v>
       </c>
-      <c r="I97" s="14" t="s">
+      <c r="I97" s="13" t="s">
         <v>56</v>
       </c>
       <c r="J97" t="s">
@@ -3555,7 +3589,7 @@
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A98" s="37" t="s">
+      <c r="A98" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B98">
@@ -3586,11 +3620,11 @@
         <f>F81+F82</f>
         <v>205</v>
       </c>
-      <c r="I98" s="14" cm="1">
+      <c r="I98" s="13" cm="1">
         <f t="array" ref="I98">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
         <v>1.1949553632967114</v>
       </c>
-      <c r="J98" s="14" cm="1">
+      <c r="J98" s="13" cm="1">
         <f t="array" ref="J98">-SUM(B99:D100*E99:G100)</f>
         <v>1.5307150056166299</v>
       </c>
@@ -3600,7 +3634,7 @@
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="37" t="s">
+      <c r="A99" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B99">
@@ -3608,11 +3642,11 @@
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="C99">
-        <f t="shared" ref="C99:D99" si="15">(D83+D84) / $F$87</f>
+        <f t="shared" ref="C99:D99" si="16">(D83+D84) / $F$87</f>
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="D99">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.06</v>
       </c>
       <c r="E99">
@@ -3631,11 +3665,11 @@
         <f>F83+F84</f>
         <v>46</v>
       </c>
-      <c r="I99" s="14" cm="1">
+      <c r="I99" s="13" cm="1">
         <f t="array" ref="I99">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
         <v>0.52330860330949647</v>
       </c>
-      <c r="J99" s="14" cm="1">
+      <c r="J99" s="13" cm="1">
         <f t="array" ref="J99">-SUM(B98:D98*E98:G98) -SUM(B100:D100*E100:G100)</f>
         <v>2.202361765603845</v>
       </c>
@@ -3645,7 +3679,7 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A100" s="37" t="s">
+      <c r="A100" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B100">
@@ -3653,11 +3687,11 @@
         <v>0.215</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:D100" si="16">(D85+D86) / $F$87</f>
+        <f t="shared" ref="C100:D100" si="17">(D85+D86) / $F$87</f>
         <v>0.03</v>
       </c>
       <c r="D100">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1275</v>
       </c>
       <c r="E100">
@@ -3676,11 +3710,11 @@
         <f>F85+F86</f>
         <v>149</v>
       </c>
-      <c r="I100" s="14" cm="1">
+      <c r="I100" s="13" cm="1">
         <f t="array" ref="I100">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
         <v>1.0074064023071336</v>
       </c>
-      <c r="J100" s="14" cm="1">
+      <c r="J100" s="13" cm="1">
         <f t="array" ref="J100">-SUM(B98:D99*E98:G99)</f>
         <v>1.7182639666062078</v>
       </c>
@@ -3690,46 +3724,46 @@
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A101" s="38" t="s">
+      <c r="A101" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="39">
+      <c r="B101" s="34">
         <f>(C81+C83+C85) / $F$87</f>
         <v>0.24249999999999999</v>
       </c>
-      <c r="C101" s="39">
-        <f t="shared" ref="C101:D101" si="17">(D81+D83+D85) / $F$87</f>
+      <c r="C101" s="34">
+        <f t="shared" ref="C101:D101" si="18">(D81+D83+D85) / $F$87</f>
         <v>0.125</v>
       </c>
-      <c r="D101" s="39">
-        <f t="shared" si="17"/>
+      <c r="D101" s="34">
+        <f t="shared" si="18"/>
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="E101" s="39">
+      <c r="E101" s="34">
         <f>LOG(Table30[[#This Row],[Proportion-Alcohol]], 2)</f>
         <v>-2.043943347587597</v>
       </c>
-      <c r="F101" s="39">
+      <c r="F101" s="34">
         <f>LOG(Table30[[#This Row],[Proportion-Cocaine]], 2)</f>
         <v>-3</v>
       </c>
-      <c r="G101" s="39">
+      <c r="G101" s="34">
         <f>LOG(Table30[[#This Row],[Proportion-Heroin]], 2)</f>
         <v>-3.3584539709124761</v>
       </c>
-      <c r="H101" s="39">
+      <c r="H101" s="34">
         <f>F81+F83+F85</f>
         <v>186</v>
       </c>
-      <c r="I101" s="40" cm="1">
+      <c r="I101" s="35" cm="1">
         <f t="array" ref="I101">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
         <v>1.1981055239539586</v>
       </c>
-      <c r="J101" s="40" cm="1">
+      <c r="J101" s="35" cm="1">
         <f t="array" ref="J101">-SUM(B102:D102 * E102:G102)</f>
         <v>1.3185974936644378</v>
       </c>
-      <c r="K101" s="39">
+      <c r="K101" s="34">
         <f>$B$95 - ((Table30[[#This Row],[Split Count]]/$F$87) * Table30[[#This Row],[Entropy-LEFT]] + (($F$87-Table30[[#This Row],[Split Count]])/$F$87) * Table30[[#This Row],[Entropy-RIGHT]])</f>
         <v>0.3036591255106067</v>
       </c>
@@ -3738,7 +3772,7 @@
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A102" s="37" t="s">
+      <c r="A102" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B102">
@@ -3746,11 +3780,11 @@
         <v>0.14749999999999999</v>
       </c>
       <c r="C102">
-        <f t="shared" ref="C102:D102" si="18">(D82+D84+D86) / $F$87</f>
+        <f t="shared" ref="C102:D102" si="19">(D82+D84+D86) / $F$87</f>
         <v>0.2225</v>
       </c>
       <c r="D102">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E102">
@@ -3769,11 +3803,11 @@
         <f>F82+F84+F86</f>
         <v>214</v>
       </c>
-      <c r="I102" s="14" cm="1">
+      <c r="I102" s="13" cm="1">
         <f t="array" ref="I102">-SUM(Table30[[#This Row],[Proportion-Alcohol]:[Proportion-Heroin]]*Table30[[#This Row],[log2(Proportion-Alcohol)]:[log2(Proportion-Heroin)]])</f>
         <v>1.3185974936644378</v>
       </c>
-      <c r="J102" s="14" cm="1">
+      <c r="J102" s="13" cm="1">
         <f t="array" ref="J102">-SUM(B101:D101 * E101:G101)</f>
         <v>1.1981055239539586</v>
       </c>
@@ -3784,38 +3818,33 @@
     </row>
     <row r="104" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="32"/>
-      <c r="B105" s="33"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="33"/>
-      <c r="E105" s="33"/>
-      <c r="F105" s="33"/>
-      <c r="G105" s="33"/>
-      <c r="H105" s="33"/>
-      <c r="I105" s="35" t="s">
+      <c r="A105" s="27"/>
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
+      <c r="I105" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J105" s="33"/>
-      <c r="K105" s="33"/>
-      <c r="L105" s="33"/>
-      <c r="M105" s="33"/>
-      <c r="N105" s="33"/>
-      <c r="O105" s="33"/>
-      <c r="P105" s="34"/>
+      <c r="J105" s="28"/>
+      <c r="K105" s="28"/>
+      <c r="L105" s="28"/>
+      <c r="M105" s="28"/>
+      <c r="N105" s="28"/>
+      <c r="O105" s="28"/>
+      <c r="P105" s="29"/>
     </row>
     <row r="106" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="31" t="s">
+      <c r="A106" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I106" s="23"/>
-      <c r="K106" s="31" t="s">
+      <c r="I106" s="19"/>
+      <c r="K106" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L106" s="10"/>
-      <c r="M106" s="10"/>
-      <c r="N106" s="10"/>
-      <c r="O106" s="10"/>
-      <c r="P106" s="10"/>
     </row>
     <row r="107" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
@@ -3836,7 +3865,7 @@
       <c r="F107" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I107" s="23"/>
+      <c r="I107" s="19"/>
       <c r="K107" s="1" t="s">
         <v>0</v>
       </c>
@@ -3876,7 +3905,7 @@
         <f>SUM(C108:E108)</f>
         <v>95</v>
       </c>
-      <c r="I108" s="23"/>
+      <c r="I108" s="19"/>
       <c r="K108" s="4" t="s">
         <v>6</v>
       </c>
@@ -3893,7 +3922,7 @@
         <v>13</v>
       </c>
       <c r="P108" s="7">
-        <f t="shared" ref="P108:P110" si="19">SUM(M108:O108)</f>
+        <f t="shared" ref="P108:P110" si="20">SUM(M108:O108)</f>
         <v>110</v>
       </c>
     </row>
@@ -3914,10 +3943,10 @@
         <v>5</v>
       </c>
       <c r="F109" s="7">
-        <f t="shared" ref="F109:F110" si="20">SUM(C109:E109)</f>
+        <f t="shared" ref="F109:F110" si="21">SUM(C109:E109)</f>
         <v>12</v>
       </c>
-      <c r="I109" s="23"/>
+      <c r="I109" s="19"/>
       <c r="K109" s="4" t="s">
         <v>9</v>
       </c>
@@ -3934,7 +3963,7 @@
         <v>19</v>
       </c>
       <c r="P109" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>34</v>
       </c>
     </row>
@@ -3955,10 +3984,10 @@
         <v>17</v>
       </c>
       <c r="F110" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>79</v>
       </c>
-      <c r="I110" s="23"/>
+      <c r="I110" s="19"/>
       <c r="K110" s="4" t="s">
         <v>10</v>
       </c>
@@ -3975,7 +4004,7 @@
         <v>34</v>
       </c>
       <c r="P110" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>70</v>
       </c>
     </row>
@@ -4000,7 +4029,7 @@
         <f>SUM(C108:E110)</f>
         <v>186</v>
       </c>
-      <c r="I111" s="23"/>
+      <c r="I111" s="19"/>
       <c r="K111" s="4" t="s">
         <v>11</v>
       </c>
@@ -4023,10 +4052,10 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I112" s="23"/>
+      <c r="I112" s="19"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I113" s="23"/>
+      <c r="I113" s="19"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
@@ -4041,7 +4070,7 @@
       <c r="D114" t="s">
         <v>48</v>
       </c>
-      <c r="I114" s="23"/>
+      <c r="I114" s="19"/>
       <c r="K114" t="s">
         <v>26</v>
       </c>
@@ -4071,7 +4100,7 @@
         <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
         <v>-0.93924596892090373</v>
       </c>
-      <c r="I115" s="23"/>
+      <c r="I115" s="19"/>
       <c r="K115" t="s">
         <v>2</v>
       </c>
@@ -4104,7 +4133,7 @@
         <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
         <v>-1.8953026213333068</v>
       </c>
-      <c r="I116" s="23"/>
+      <c r="I116" s="19"/>
       <c r="K116" t="s">
         <v>3</v>
       </c>
@@ -4137,7 +4166,7 @@
         <f>LOG(Table2934[[#This Row],[Proportion]], 2)</f>
         <v>-2.2537565922457832</v>
       </c>
-      <c r="I117" s="23"/>
+      <c r="I117" s="19"/>
       <c r="K117" t="s">
         <v>4</v>
       </c>
@@ -4155,30 +4184,30 @@
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I118" s="23"/>
+      <c r="I118" s="19"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B119" s="13" cm="1">
+      <c r="B119" s="12" cm="1">
         <f t="array" ref="B119">-SUM(Table2934[Proportion] * Table2934[log2(Proportion)])</f>
         <v>1.4718736405891319</v>
       </c>
-      <c r="I119" s="23"/>
-      <c r="K119" s="12" t="s">
+      <c r="I119" s="19"/>
+      <c r="K119" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L119" s="13" cm="1">
+      <c r="L119" s="12" cm="1">
         <f t="array" ref="L119">-SUM(Table293437[Proportion] * Table293437[log2(Proportion)])</f>
         <v>1.5622790090833154</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I120" s="23"/>
+      <c r="I120" s="19"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A121" s="37" t="s">
+      <c r="A121" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B121" t="s">
@@ -4202,8 +4231,8 @@
       <c r="H121" t="s">
         <v>58</v>
       </c>
-      <c r="I121" s="23"/>
-      <c r="K121" s="37" t="s">
+      <c r="I121" s="19"/>
+      <c r="K121" s="32" t="s">
         <v>28</v>
       </c>
       <c r="L121" t="s">
@@ -4229,7 +4258,7 @@
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A122" s="37" t="s">
+      <c r="A122" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B122">
@@ -4237,11 +4266,11 @@
         <v>0.16129032258064516</v>
       </c>
       <c r="C122">
-        <f t="shared" ref="C122:D122" si="21">D108/$F$111</f>
+        <f t="shared" ref="C122:D122" si="22">D108/$F$111</f>
         <v>0.25806451612903225</v>
       </c>
       <c r="D122">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.1397849462365593E-2</v>
       </c>
       <c r="E122">
@@ -4260,8 +4289,8 @@
         <f>F108</f>
         <v>95</v>
       </c>
-      <c r="I122" s="23"/>
-      <c r="K122" s="37" t="s">
+      <c r="I122" s="19"/>
+      <c r="K122" s="32" t="s">
         <v>6</v>
       </c>
       <c r="L122">
@@ -4269,11 +4298,11 @@
         <v>0.11682242990654206</v>
       </c>
       <c r="M122">
-        <f t="shared" ref="M122:N122" si="22">N108/$P$111</f>
+        <f t="shared" ref="M122:N122" si="23">N108/$P$111</f>
         <v>0.3364485981308411</v>
       </c>
       <c r="N122">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6.0747663551401869E-2</v>
       </c>
       <c r="O122">
@@ -4294,7 +4323,7 @@
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A123" s="37" t="s">
+      <c r="A123" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B123">
@@ -4302,11 +4331,11 @@
         <v>3.7634408602150539E-2</v>
       </c>
       <c r="C123">
-        <f t="shared" ref="C123:D123" si="23">D109/$F$111</f>
+        <f t="shared" ref="C123:D123" si="24">D109/$F$111</f>
         <v>0</v>
       </c>
       <c r="D123">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.6881720430107527E-2</v>
       </c>
       <c r="E123">
@@ -4321,23 +4350,23 @@
         <v>-5.2172307162206693</v>
       </c>
       <c r="H123">
-        <f t="shared" ref="H123:H124" si="24">F109</f>
+        <f t="shared" ref="H123:H124" si="25">F109</f>
         <v>12</v>
       </c>
-      <c r="I123" s="23"/>
-      <c r="K123" s="37" t="s">
+      <c r="I123" s="19"/>
+      <c r="K123" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L123">
-        <f t="shared" ref="L123:N123" si="25">M109/$P$111</f>
+        <f t="shared" ref="L123:N123" si="26">M109/$P$111</f>
         <v>3.7383177570093455E-2</v>
       </c>
       <c r="M123">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.2710280373831772E-2</v>
       </c>
       <c r="N123">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>8.8785046728971959E-2</v>
       </c>
       <c r="O123">
@@ -4352,12 +4381,12 @@
         <v>-3.4935394729575613</v>
       </c>
       <c r="R123">
-        <f t="shared" ref="R123:R124" si="26">P109</f>
+        <f t="shared" ref="R123:R124" si="27">P109</f>
         <v>34</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A124" s="37" t="s">
+      <c r="A124" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B124">
@@ -4365,11 +4394,11 @@
         <v>0.32258064516129031</v>
       </c>
       <c r="C124">
-        <f t="shared" ref="C124:D124" si="27">D110/$F$111</f>
+        <f t="shared" ref="C124:D124" si="28">D110/$F$111</f>
         <v>1.0752688172043012E-2</v>
       </c>
       <c r="D124">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>9.1397849462365593E-2</v>
       </c>
       <c r="E124">
@@ -4385,23 +4414,23 @@
         <v>-3.4516959698576919</v>
       </c>
       <c r="H124">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>79</v>
       </c>
-      <c r="I124" s="23"/>
-      <c r="K124" s="37" t="s">
+      <c r="I124" s="19"/>
+      <c r="K124" s="32" t="s">
         <v>10</v>
       </c>
       <c r="L124">
-        <f t="shared" ref="L124:N124" si="28">M110/$P$111</f>
+        <f t="shared" ref="L124:N124" si="29">M110/$P$111</f>
         <v>0.12149532710280374</v>
       </c>
       <c r="M124">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4.6728971962616821E-2</v>
       </c>
       <c r="N124">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.15887850467289719</v>
       </c>
       <c r="O124">
@@ -4417,72 +4446,72 @@
         <v>-2.6540041451508074</v>
       </c>
       <c r="R124">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>70</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I125" s="23"/>
+      <c r="I125" s="19"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B126" s="42" t="s">
+      <c r="B126" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C126" s="43" t="s">
+      <c r="C126" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D126" s="43" t="s">
+      <c r="D126" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="I126" s="23"/>
-      <c r="K126" s="41" t="s">
+      <c r="I126" s="19"/>
+      <c r="K126" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="L126" s="42" t="s">
+      <c r="L126" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="M126" s="43" t="s">
+      <c r="M126" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="N126" s="43" t="s">
+      <c r="N126" s="38" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A127" s="49" t="s">
+      <c r="A127" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B127" s="50" cm="1">
+      <c r="B127" s="45" cm="1">
         <f t="array" ref="B127">-SUM(B122:D122*E122:G122)</f>
         <v>1.2443457035007321</v>
       </c>
-      <c r="C127" s="50" cm="1">
+      <c r="C127" s="45" cm="1">
         <f t="array" ref="C127">-SUM(B123:D124*E123:G124)</f>
         <v>1.2306560367969031</v>
       </c>
-      <c r="D127" s="51">
+      <c r="D127" s="46">
         <f>$B$119 - ((H122/$F$111) * B127 + (($F$111-H122)/$F$111) * C127)</f>
         <v>0.23422556972306885</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I127" s="23"/>
-      <c r="K127" s="52" t="s">
+      <c r="I127" s="19"/>
+      <c r="K127" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="L127" s="53" cm="1">
+      <c r="L127" s="48" cm="1">
         <f t="array" ref="L127">-SUM(L122:N122*O122:Q122)</f>
         <v>1.1360964828040998</v>
       </c>
-      <c r="M127" s="53" cm="1">
+      <c r="M127" s="48" cm="1">
         <f t="array" ref="M127">-SUM(L123:N124*O123:Q124)</f>
         <v>1.4850804892636895</v>
       </c>
-      <c r="N127" s="54">
+      <c r="N127" s="49">
         <f>$L$119 - ((R122/$P$111) * L127 + (($P$111-R122)/$P$111) * M127)</f>
         <v>0.2565828222053963</v>
       </c>
@@ -4491,115 +4520,110 @@
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A128" s="46" t="s">
+      <c r="A128" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B128" s="47" cm="1">
+      <c r="B128" s="42" cm="1">
         <f t="array" ref="B128">-SUM(B123:D123*E123:G123)</f>
         <v>0.31832677851858249</v>
       </c>
-      <c r="C128" s="47" cm="1">
+      <c r="C128" s="42" cm="1">
         <f t="array" ref="C128">-SUM(B122:D122*E122:G122) -SUM(B124:D124*E124:G124)</f>
         <v>2.1566749617790526</v>
       </c>
-      <c r="D128" s="48">
-        <f t="shared" ref="D128:D129" si="29">$B$119 - ((H123/$F$111) * B128 + (($F$111-H123)/$F$111) * C128)</f>
+      <c r="D128" s="43">
+        <f t="shared" ref="D128:D129" si="30">$B$119 - ((H123/$F$111) * B128 + (($F$111-H123)/$F$111) * C128)</f>
         <v>-0.56619821259247116</v>
       </c>
-      <c r="I128" s="23"/>
-      <c r="K128" s="46" t="s">
+      <c r="I128" s="19"/>
+      <c r="K128" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L128" s="47" cm="1">
+      <c r="L128" s="42" cm="1">
         <f t="array" ref="L128">-SUM(L123:N123*O123:Q123)</f>
         <v>0.48742516765141508</v>
       </c>
-      <c r="M128" s="47" cm="1">
+      <c r="M128" s="42" cm="1">
         <f t="array" ref="M128">-SUM(L122:N122*O122:Q122) -SUM(L124:N124*O124:Q124)</f>
         <v>2.1337518044163741</v>
       </c>
-      <c r="N128" s="48">
+      <c r="N128" s="43">
         <f>$L$119 - ((R123/$P$111) * L128 + (($P$111-R123)/$P$111) * M128)</f>
         <v>-0.30990688108068198</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A129" s="44" t="s">
+      <c r="A129" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B129" s="45" cm="1">
+      <c r="B129" s="40" cm="1">
         <f t="array" ref="B129">-SUM(B124:D124*E124:G124)</f>
         <v>0.91232925827832045</v>
       </c>
-      <c r="C129" s="45" cm="1">
+      <c r="C129" s="40" cm="1">
         <f t="array" ref="C129">-SUM(B122:D123*E122:G123)</f>
         <v>1.5626724820193147</v>
       </c>
-      <c r="D129" s="48">
-        <f t="shared" si="29"/>
+      <c r="D129" s="43">
+        <f t="shared" si="30"/>
         <v>0.18542220521249742</v>
       </c>
-      <c r="I129" s="23"/>
-      <c r="K129" s="44" t="s">
+      <c r="I129" s="19"/>
+      <c r="K129" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L129" s="45" cm="1">
+      <c r="L129" s="40" cm="1">
         <f t="array" ref="L129">-SUM(L124:N124*O124:Q124)</f>
         <v>0.99765532161227433</v>
       </c>
-      <c r="M129" s="45" cm="1">
+      <c r="M129" s="40" cm="1">
         <f t="array" ref="M129">-SUM(L122:N123*O122:Q123)</f>
         <v>1.623521650455515</v>
       </c>
-      <c r="N129" s="11">
-        <f t="shared" ref="N129" si="30">$L$119 - ((R124/$P$111) * L129 + (($P$111-R124)/$P$111) * M129)</f>
+      <c r="N129" s="10">
+        <f t="shared" ref="N129" si="31">$L$119 - ((R124/$P$111) * L129 + (($P$111-R124)/$P$111) * M129)</f>
         <v>0.14347998955783248</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I130" s="23"/>
+      <c r="I130" s="19"/>
     </row>
     <row r="131" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I131" s="23"/>
+      <c r="I131" s="19"/>
     </row>
     <row r="132" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="23"/>
-      <c r="B132" s="23"/>
-      <c r="C132" s="23"/>
-      <c r="D132" s="23"/>
-      <c r="E132" s="23"/>
-      <c r="F132" s="23"/>
-      <c r="G132" s="23"/>
-      <c r="H132" s="23"/>
-      <c r="I132" s="36" t="s">
+      <c r="A132" s="19"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="J132" s="23"/>
-      <c r="K132" s="23"/>
-      <c r="L132" s="23"/>
-      <c r="M132" s="23"/>
-      <c r="N132" s="23"/>
-      <c r="O132" s="23"/>
-      <c r="P132" s="23"/>
-      <c r="Q132" s="23"/>
-      <c r="R132" s="23"/>
+      <c r="J132" s="19"/>
+      <c r="K132" s="19"/>
+      <c r="L132" s="19"/>
+      <c r="M132" s="19"/>
+      <c r="N132" s="19"/>
+      <c r="O132" s="19"/>
+      <c r="P132" s="19"/>
+      <c r="Q132" s="19"/>
+      <c r="R132" s="19"/>
     </row>
     <row r="133" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I133" s="23"/>
+      <c r="I133" s="19"/>
     </row>
     <row r="134" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="24" t="s">
+      <c r="A134" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I134" s="23"/>
-      <c r="K134" s="24" t="s">
+      <c r="I134" s="19"/>
+      <c r="K134" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L134" s="10"/>
-      <c r="M134" s="10"/>
-      <c r="N134" s="10"/>
-      <c r="O134" s="10"/>
-      <c r="P134" s="10"/>
     </row>
     <row r="135" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
@@ -4611,7 +4635,7 @@
       <c r="C135" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D135" s="29" t="s">
+      <c r="D135" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E135" s="3" t="s">
@@ -4620,7 +4644,7 @@
       <c r="F135" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I135" s="23"/>
+      <c r="I135" s="19"/>
       <c r="K135" s="1" t="s">
         <v>0</v>
       </c>
@@ -4630,7 +4654,7 @@
       <c r="M135" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N135" s="29" t="s">
+      <c r="N135" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O135" s="3" t="s">
@@ -4650,7 +4674,7 @@
       <c r="C136" s="6">
         <v>30</v>
       </c>
-      <c r="D136" s="22">
+      <c r="D136" s="18">
         <v>48</v>
       </c>
       <c r="E136" s="6">
@@ -4660,7 +4684,10 @@
         <f>SUM(C136:E136)</f>
         <v>95</v>
       </c>
-      <c r="I136" s="23"/>
+      <c r="G136" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I136" s="19"/>
       <c r="K136" s="4" t="s">
         <v>6</v>
       </c>
@@ -4670,15 +4697,18 @@
       <c r="M136" s="6">
         <v>25</v>
       </c>
-      <c r="N136" s="22">
+      <c r="N136" s="18">
         <v>72</v>
       </c>
       <c r="O136" s="6">
         <v>13</v>
       </c>
       <c r="P136" s="7">
-        <f t="shared" ref="P136" si="31">SUM(M136:O136)</f>
+        <f t="shared" ref="P136" si="32">SUM(M136:O136)</f>
         <v>110</v>
+      </c>
+      <c r="Q136" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="137" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -4690,7 +4720,7 @@
         <f>SUM(C136:C136)</f>
         <v>30</v>
       </c>
-      <c r="D137" s="22">
+      <c r="D137" s="18">
         <f>SUM(D136:D136)</f>
         <v>48</v>
       </c>
@@ -4702,7 +4732,7 @@
         <f>SUM(C136:E136)</f>
         <v>95</v>
       </c>
-      <c r="I137" s="23"/>
+      <c r="I137" s="19"/>
       <c r="K137" s="4" t="s">
         <v>11</v>
       </c>
@@ -4711,7 +4741,7 @@
         <f>SUM(M136:M136)</f>
         <v>25</v>
       </c>
-      <c r="N137" s="22">
+      <c r="N137" s="18">
         <f>SUM(N136:N136)</f>
         <v>72</v>
       </c>
@@ -4725,21 +4755,16 @@
       </c>
     </row>
     <row r="138" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I138" s="23"/>
+      <c r="I138" s="19"/>
     </row>
     <row r="139" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I139" s="23"/>
-      <c r="K139" s="24" t="s">
+      <c r="I139" s="19"/>
+      <c r="K139" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="L139" s="10"/>
-      <c r="M139" s="10"/>
-      <c r="N139" s="10"/>
-      <c r="O139" s="10"/>
-      <c r="P139" s="10"/>
     </row>
     <row r="140" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
@@ -4748,7 +4773,7 @@
       <c r="B140" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C140" s="29" t="s">
+      <c r="C140" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D140" s="3" t="s">
@@ -4760,7 +4785,7 @@
       <c r="F140" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I140" s="23"/>
+      <c r="I140" s="19"/>
       <c r="K140" s="1" t="s">
         <v>0</v>
       </c>
@@ -4773,7 +4798,7 @@
       <c r="N140" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O140" s="29" t="s">
+      <c r="O140" s="24" t="s">
         <v>4</v>
       </c>
       <c r="P140" s="3" t="s">
@@ -4787,7 +4812,7 @@
       <c r="B141" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C141" s="22">
+      <c r="C141" s="18">
         <v>7</v>
       </c>
       <c r="D141" s="6">
@@ -4797,10 +4822,13 @@
         <v>5</v>
       </c>
       <c r="F141" s="7">
-        <f t="shared" ref="F141:F142" si="32">SUM(C141:E141)</f>
+        <f t="shared" ref="F141:F142" si="33">SUM(C141:E141)</f>
         <v>12</v>
       </c>
-      <c r="I141" s="23"/>
+      <c r="G141" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I141" s="19"/>
       <c r="K141" s="4" t="s">
         <v>9</v>
       </c>
@@ -4813,12 +4841,15 @@
       <c r="N141" s="6">
         <v>7</v>
       </c>
-      <c r="O141" s="22">
+      <c r="O141" s="18">
         <v>19</v>
       </c>
       <c r="P141" s="7">
-        <f t="shared" ref="P141:P142" si="33">SUM(M141:O141)</f>
+        <f t="shared" ref="P141:P142" si="34">SUM(M141:O141)</f>
         <v>34</v>
+      </c>
+      <c r="Q141" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="142" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -4828,7 +4859,7 @@
       <c r="B142" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C142" s="22">
+      <c r="C142" s="18">
         <v>60</v>
       </c>
       <c r="D142" s="6">
@@ -4838,10 +4869,13 @@
         <v>17</v>
       </c>
       <c r="F142" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>79</v>
       </c>
-      <c r="I142" s="23"/>
+      <c r="G142" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I142" s="19"/>
       <c r="K142" s="4" t="s">
         <v>10</v>
       </c>
@@ -4854,12 +4888,15 @@
       <c r="N142" s="6">
         <v>10</v>
       </c>
-      <c r="O142" s="22">
+      <c r="O142" s="18">
         <v>34</v>
       </c>
       <c r="P142" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>70</v>
+      </c>
+      <c r="Q142" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="143" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -4867,7 +4904,7 @@
         <v>11</v>
       </c>
       <c r="B143" s="5"/>
-      <c r="C143" s="22">
+      <c r="C143" s="18">
         <f>SUM(C141:C142)</f>
         <v>67</v>
       </c>
@@ -4883,7 +4920,7 @@
         <f>SUM(C141:E142)</f>
         <v>91</v>
       </c>
-      <c r="I143" s="23"/>
+      <c r="I143" s="19"/>
       <c r="K143" s="4" t="s">
         <v>11</v>
       </c>
@@ -4896,7 +4933,7 @@
         <f>SUM(N141:N142)</f>
         <v>17</v>
       </c>
-      <c r="O143" s="22">
+      <c r="O143" s="18">
         <f>SUM(O141:O142)</f>
         <v>53</v>
       </c>
@@ -4906,31 +4943,31 @@
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I144" s="23"/>
+      <c r="I144" s="19"/>
     </row>
     <row r="145" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I145" s="23"/>
+      <c r="I145" s="19"/>
     </row>
     <row r="146" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="32"/>
-      <c r="B146" s="33"/>
-      <c r="C146" s="33"/>
-      <c r="D146" s="33"/>
-      <c r="E146" s="33"/>
-      <c r="F146" s="33"/>
-      <c r="G146" s="33"/>
-      <c r="H146" s="33"/>
-      <c r="I146" s="33"/>
-      <c r="J146" s="33"/>
-      <c r="K146" s="33"/>
-      <c r="L146" s="33"/>
-      <c r="M146" s="33"/>
-      <c r="N146" s="33"/>
-      <c r="O146" s="33"/>
-      <c r="P146" s="34"/>
+      <c r="A146" s="27"/>
+      <c r="B146" s="28"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="28"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="28"/>
+      <c r="G146" s="28"/>
+      <c r="H146" s="28"/>
+      <c r="I146" s="28"/>
+      <c r="J146" s="28"/>
+      <c r="K146" s="28"/>
+      <c r="L146" s="28"/>
+      <c r="M146" s="28"/>
+      <c r="N146" s="28"/>
+      <c r="O146" s="28"/>
+      <c r="P146" s="29"/>
     </row>
     <row r="147" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="31" t="s">
+      <c r="A147" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4965,7 +5002,7 @@
       <c r="B151" t="s">
         <v>2</v>
       </c>
-      <c r="C151" s="55" t="s">
+      <c r="C151" s="50" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>